<commit_message>
[docs] update threat number & risk assessment
update threat number & risk assessment
move some document files
</commit_message>
<xml_diff>
--- a/docs/05_threat_modeling/threat_modeling.xlsx
+++ b/docs/05_threat_modeling/threat_modeling.xlsx
@@ -9,18 +9,18 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12390" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12390"/>
   </bookViews>
   <sheets>
     <sheet name="threat_modeling_all" sheetId="1" r:id="rId1"/>
-    <sheet name="risk_assessment" sheetId="2" r:id="rId2"/>
+    <sheet name="threat_list" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="577" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="662" uniqueCount="273">
   <si>
     <t>Id</t>
   </si>
@@ -641,6 +641,391 @@
   <si>
     <t xml:space="preserve">
 The number of images should be under 100.</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">If the user credential data is stored as plain text, it can be disclosed. </t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>DF4.2 Load Login Credential / Learning Data ...</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Information Disclosure</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Tampering</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>An attacker modify user credential data and then server can use it without checking.</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Spoofing</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>DF2.1 Reqest (Login / Mode Ctrl..)</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>An attacker spoof the user (Client)</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Spoofing</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Repudiation</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Clients can repudiate the actions they have performed.</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Information Disclosure</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>An attack can sniff the data on the connection.</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Information Disclosure</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Weak Authentification may lead to disclose information</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Denial Of Service</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>the information of the communication between client and server is interrupted by attackers.</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Elevation Of Privilege</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>DF3.1 Camera Ctrl</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>It may be physically damaged and you may not be able to get Data from Camera</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>DF4.1 Store Login Credential / Learning Data ...</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>It is possible to add a lot of Images in the storage.</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>User credential may be disclosed.</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>DF2.5 Result (Video Stream...)</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Client (PC) may be spoofed by an attacker </t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Tampering</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Video Stream may be tampered with by an attacker.</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Video Stream may be sniffed with by an attacker.</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Denial Of Service</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Tampering</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Change the image data not to recognize registered users.</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Information Disclosure</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sniff the communication channel between server and client to get user credential data.</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Network</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Compromise the connection of network physically by an attacker</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>TR-01</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>TR-02</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>TR-03</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>TR-04</t>
+  </si>
+  <si>
+    <t>TR-05</t>
+  </si>
+  <si>
+    <t>TR-06</t>
+  </si>
+  <si>
+    <t>TR-07</t>
+  </si>
+  <si>
+    <t>TR-08</t>
+  </si>
+  <si>
+    <t>TR-09</t>
+  </si>
+  <si>
+    <t>TR-10</t>
+  </si>
+  <si>
+    <t>TR-11</t>
+  </si>
+  <si>
+    <t>TR-12</t>
+  </si>
+  <si>
+    <t>TR-13</t>
+  </si>
+  <si>
+    <t>TR-14</t>
+  </si>
+  <si>
+    <t>TR-15</t>
+  </si>
+  <si>
+    <t>TR-16</t>
+  </si>
+  <si>
+    <t>TR-17</t>
+  </si>
+  <si>
+    <t>TR-18</t>
+  </si>
+  <si>
+    <t>TR-19</t>
+  </si>
+  <si>
+    <t>TR-20</t>
+  </si>
+  <si>
+    <t>TR-21</t>
+  </si>
+  <si>
+    <t>TR-22</t>
+  </si>
+  <si>
+    <t>TR-23</t>
+  </si>
+  <si>
+    <t>TR-24</t>
+  </si>
+  <si>
+    <t>TR-25</t>
+  </si>
+  <si>
+    <t>TR-26</t>
+  </si>
+  <si>
+    <t>TR-27</t>
+  </si>
+  <si>
+    <t>TR-28</t>
+  </si>
+  <si>
+    <t>TR-29</t>
+  </si>
+  <si>
+    <t>TR-30</t>
+  </si>
+  <si>
+    <t>TR-31</t>
+  </si>
+  <si>
+    <t>TR-32</t>
+  </si>
+  <si>
+    <t>TR-33</t>
+  </si>
+  <si>
+    <t>TR-34</t>
+  </si>
+  <si>
+    <t>TR-35</t>
+  </si>
+  <si>
+    <t>TR-36</t>
+  </si>
+  <si>
+    <t>TR-37</t>
+  </si>
+  <si>
+    <t>TR-38</t>
+  </si>
+  <si>
+    <t>TR-39</t>
+  </si>
+  <si>
+    <t>TR-40</t>
+  </si>
+  <si>
+    <t>TR-41</t>
+  </si>
+  <si>
+    <t>TR-42</t>
+  </si>
+  <si>
+    <t>TR-43</t>
+  </si>
+  <si>
+    <t>TR-44</t>
+  </si>
+  <si>
+    <t>TR-45</t>
+  </si>
+  <si>
+    <t>TR-46</t>
+  </si>
+  <si>
+    <t>TR-47</t>
+  </si>
+  <si>
+    <t>TR-48</t>
+  </si>
+  <si>
+    <t>TR-49</t>
+  </si>
+  <si>
+    <t>TR-50</t>
+  </si>
+  <si>
+    <t>TR-51</t>
+  </si>
+  <si>
+    <t>TR-52</t>
+  </si>
+  <si>
+    <t>TR-53</t>
+  </si>
+  <si>
+    <t>TR-54</t>
+  </si>
+  <si>
+    <t>TR-55</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>TR-56</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>TR-57</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>TR-58</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>TR-59</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>TR-60</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>TR-10</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>TR-13</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>TR-29</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>TR-34</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>TR-35</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>TR-41</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>TR-44</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>TR-45</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>TR-46</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>TR-48</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>TR-49</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>TR-52</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>TR-53</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>TR-59</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -1696,14 +2081,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H63"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C17" sqref="C17"/>
+      <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.75" customWidth="1"/>
     <col min="2" max="2" width="13.75" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="21.875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="36.125" customWidth="1"/>
@@ -1740,8 +2125,8 @@
       </c>
     </row>
     <row r="2" spans="1:8" s="3" customFormat="1" ht="33" x14ac:dyDescent="0.3">
-      <c r="A2" s="7">
-        <v>1</v>
+      <c r="A2" s="7" t="s">
+        <v>199</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>129</v>
@@ -1764,8 +2149,8 @@
       </c>
     </row>
     <row r="3" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="7">
-        <v>2</v>
+      <c r="A3" s="7" t="s">
+        <v>200</v>
       </c>
       <c r="B3" s="7" t="s">
         <v>129</v>
@@ -1788,8 +2173,8 @@
       </c>
     </row>
     <row r="4" spans="1:8" s="2" customFormat="1" ht="33" x14ac:dyDescent="0.3">
-      <c r="A4" s="7">
-        <v>3</v>
+      <c r="A4" s="7" t="s">
+        <v>201</v>
       </c>
       <c r="B4" s="7" t="s">
         <v>129</v>
@@ -1812,8 +2197,8 @@
       </c>
     </row>
     <row r="5" spans="1:8" s="2" customFormat="1" ht="33" x14ac:dyDescent="0.3">
-      <c r="A5" s="7">
-        <v>4</v>
+      <c r="A5" s="7" t="s">
+        <v>202</v>
       </c>
       <c r="B5" s="7" t="s">
         <v>129</v>
@@ -1836,8 +2221,8 @@
       </c>
     </row>
     <row r="6" spans="1:8" s="2" customFormat="1" ht="33" x14ac:dyDescent="0.3">
-      <c r="A6" s="7">
-        <v>5</v>
+      <c r="A6" s="7" t="s">
+        <v>203</v>
       </c>
       <c r="B6" s="7" t="s">
         <v>129</v>
@@ -1860,8 +2245,8 @@
       </c>
     </row>
     <row r="7" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="7">
-        <v>6</v>
+      <c r="A7" s="7" t="s">
+        <v>204</v>
       </c>
       <c r="B7" s="7" t="s">
         <v>129</v>
@@ -1884,8 +2269,8 @@
       </c>
     </row>
     <row r="8" spans="1:8" s="2" customFormat="1" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="A8" s="7">
-        <v>7</v>
+      <c r="A8" s="7" t="s">
+        <v>205</v>
       </c>
       <c r="B8" s="7" t="s">
         <v>129</v>
@@ -1908,8 +2293,8 @@
       </c>
     </row>
     <row r="9" spans="1:8" s="2" customFormat="1" ht="33" x14ac:dyDescent="0.3">
-      <c r="A9" s="7">
-        <v>8</v>
+      <c r="A9" s="7" t="s">
+        <v>206</v>
       </c>
       <c r="B9" s="7" t="s">
         <v>129</v>
@@ -1932,8 +2317,8 @@
       </c>
     </row>
     <row r="10" spans="1:8" s="10" customFormat="1" ht="33" x14ac:dyDescent="0.3">
-      <c r="A10" s="9">
-        <v>9</v>
+      <c r="A10" s="9" t="s">
+        <v>207</v>
       </c>
       <c r="B10" s="8" t="s">
         <v>129</v>
@@ -1958,8 +2343,8 @@
       </c>
     </row>
     <row r="11" spans="1:8" s="2" customFormat="1" ht="33" x14ac:dyDescent="0.3">
-      <c r="A11" s="7">
-        <v>10</v>
+      <c r="A11" s="7" t="s">
+        <v>208</v>
       </c>
       <c r="B11" s="7" t="s">
         <v>129</v>
@@ -1982,8 +2367,8 @@
       </c>
     </row>
     <row r="12" spans="1:8" s="10" customFormat="1" ht="33" x14ac:dyDescent="0.3">
-      <c r="A12" s="9">
-        <v>11</v>
+      <c r="A12" s="9" t="s">
+        <v>209</v>
       </c>
       <c r="B12" s="8" t="s">
         <v>129</v>
@@ -2008,8 +2393,8 @@
       </c>
     </row>
     <row r="13" spans="1:8" s="10" customFormat="1" ht="33" x14ac:dyDescent="0.3">
-      <c r="A13" s="9">
-        <v>12</v>
+      <c r="A13" s="9" t="s">
+        <v>210</v>
       </c>
       <c r="B13" s="8" t="s">
         <v>129</v>
@@ -2034,8 +2419,8 @@
       </c>
     </row>
     <row r="14" spans="1:8" s="2" customFormat="1" ht="33" x14ac:dyDescent="0.3">
-      <c r="A14" s="7">
-        <v>13</v>
+      <c r="A14" s="7" t="s">
+        <v>211</v>
       </c>
       <c r="B14" s="7" t="s">
         <v>129</v>
@@ -2060,8 +2445,8 @@
       </c>
     </row>
     <row r="15" spans="1:8" s="10" customFormat="1" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="A15" s="9">
-        <v>14</v>
+      <c r="A15" s="9" t="s">
+        <v>212</v>
       </c>
       <c r="B15" s="8" t="s">
         <v>129</v>
@@ -2086,8 +2471,8 @@
       </c>
     </row>
     <row r="16" spans="1:8" s="10" customFormat="1" ht="33" x14ac:dyDescent="0.3">
-      <c r="A16" s="9">
-        <v>15</v>
+      <c r="A16" s="9" t="s">
+        <v>213</v>
       </c>
       <c r="B16" s="8" t="s">
         <v>129</v>
@@ -2112,8 +2497,8 @@
       </c>
     </row>
     <row r="17" spans="1:8" s="10" customFormat="1" ht="66" x14ac:dyDescent="0.3">
-      <c r="A17" s="9">
-        <v>16</v>
+      <c r="A17" s="9" t="s">
+        <v>214</v>
       </c>
       <c r="B17" s="8" t="s">
         <v>129</v>
@@ -2138,8 +2523,8 @@
       </c>
     </row>
     <row r="18" spans="1:8" s="10" customFormat="1" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="A18" s="9">
-        <v>17</v>
+      <c r="A18" s="9" t="s">
+        <v>215</v>
       </c>
       <c r="B18" s="8" t="s">
         <v>129</v>
@@ -2164,8 +2549,8 @@
       </c>
     </row>
     <row r="19" spans="1:8" s="10" customFormat="1" ht="82.5" x14ac:dyDescent="0.3">
-      <c r="A19" s="9">
-        <v>18</v>
+      <c r="A19" s="9" t="s">
+        <v>216</v>
       </c>
       <c r="B19" s="8" t="s">
         <v>129</v>
@@ -2190,8 +2575,8 @@
       </c>
     </row>
     <row r="20" spans="1:8" s="10" customFormat="1" ht="33" x14ac:dyDescent="0.3">
-      <c r="A20" s="9">
-        <v>19</v>
+      <c r="A20" s="9" t="s">
+        <v>217</v>
       </c>
       <c r="B20" s="8" t="s">
         <v>129</v>
@@ -2216,8 +2601,8 @@
       </c>
     </row>
     <row r="21" spans="1:8" s="10" customFormat="1" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="A21" s="9">
-        <v>20</v>
+      <c r="A21" s="9" t="s">
+        <v>218</v>
       </c>
       <c r="B21" s="8" t="s">
         <v>129</v>
@@ -2242,8 +2627,8 @@
       </c>
     </row>
     <row r="22" spans="1:8" s="10" customFormat="1" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="A22" s="9">
-        <v>21</v>
+      <c r="A22" s="9" t="s">
+        <v>219</v>
       </c>
       <c r="B22" s="8" t="s">
         <v>129</v>
@@ -2268,8 +2653,8 @@
       </c>
     </row>
     <row r="23" spans="1:8" s="10" customFormat="1" ht="33" x14ac:dyDescent="0.3">
-      <c r="A23" s="9">
-        <v>22</v>
+      <c r="A23" s="9" t="s">
+        <v>220</v>
       </c>
       <c r="B23" s="8" t="s">
         <v>129</v>
@@ -2294,8 +2679,8 @@
       </c>
     </row>
     <row r="24" spans="1:8" s="10" customFormat="1" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="A24" s="9">
-        <v>23</v>
+      <c r="A24" s="9" t="s">
+        <v>221</v>
       </c>
       <c r="B24" s="8" t="s">
         <v>129</v>
@@ -2320,8 +2705,8 @@
       </c>
     </row>
     <row r="25" spans="1:8" s="10" customFormat="1" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="A25" s="9">
-        <v>24</v>
+      <c r="A25" s="9" t="s">
+        <v>222</v>
       </c>
       <c r="B25" s="8" t="s">
         <v>129</v>
@@ -2346,8 +2731,8 @@
       </c>
     </row>
     <row r="26" spans="1:8" s="10" customFormat="1" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="A26" s="9">
-        <v>25</v>
+      <c r="A26" s="9" t="s">
+        <v>223</v>
       </c>
       <c r="B26" s="8" t="s">
         <v>129</v>
@@ -2372,8 +2757,8 @@
       </c>
     </row>
     <row r="27" spans="1:8" s="10" customFormat="1" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="A27" s="9">
-        <v>26</v>
+      <c r="A27" s="9" t="s">
+        <v>224</v>
       </c>
       <c r="B27" s="8" t="s">
         <v>129</v>
@@ -2398,8 +2783,8 @@
       </c>
     </row>
     <row r="28" spans="1:8" s="10" customFormat="1" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="A28" s="9">
-        <v>27</v>
+      <c r="A28" s="9" t="s">
+        <v>225</v>
       </c>
       <c r="B28" s="8" t="s">
         <v>129</v>
@@ -2424,8 +2809,8 @@
       </c>
     </row>
     <row r="29" spans="1:8" s="10" customFormat="1" ht="82.5" x14ac:dyDescent="0.3">
-      <c r="A29" s="9">
-        <v>28</v>
+      <c r="A29" s="9" t="s">
+        <v>226</v>
       </c>
       <c r="B29" s="8" t="s">
         <v>129</v>
@@ -2450,8 +2835,8 @@
       </c>
     </row>
     <row r="30" spans="1:8" s="2" customFormat="1" ht="33" x14ac:dyDescent="0.3">
-      <c r="A30" s="7">
-        <v>29</v>
+      <c r="A30" s="7" t="s">
+        <v>227</v>
       </c>
       <c r="B30" s="6" t="s">
         <v>129</v>
@@ -2476,8 +2861,8 @@
       </c>
     </row>
     <row r="31" spans="1:8" s="10" customFormat="1" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="A31" s="9">
-        <v>30</v>
+      <c r="A31" s="9" t="s">
+        <v>228</v>
       </c>
       <c r="B31" s="8" t="s">
         <v>129</v>
@@ -2502,8 +2887,8 @@
       </c>
     </row>
     <row r="32" spans="1:8" s="10" customFormat="1" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="A32" s="9">
-        <v>31</v>
+      <c r="A32" s="9" t="s">
+        <v>229</v>
       </c>
       <c r="B32" s="8" t="s">
         <v>129</v>
@@ -2528,8 +2913,8 @@
       </c>
     </row>
     <row r="33" spans="1:8" s="10" customFormat="1" ht="33" x14ac:dyDescent="0.3">
-      <c r="A33" s="9">
-        <v>32</v>
+      <c r="A33" s="9" t="s">
+        <v>230</v>
       </c>
       <c r="B33" s="8" t="s">
         <v>129</v>
@@ -2554,8 +2939,8 @@
       </c>
     </row>
     <row r="34" spans="1:8" s="10" customFormat="1" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="A34" s="9">
-        <v>33</v>
+      <c r="A34" s="9" t="s">
+        <v>231</v>
       </c>
       <c r="B34" s="8" t="s">
         <v>129</v>
@@ -2580,8 +2965,8 @@
       </c>
     </row>
     <row r="35" spans="1:8" s="2" customFormat="1" ht="33" x14ac:dyDescent="0.3">
-      <c r="A35" s="7">
-        <v>34</v>
+      <c r="A35" s="7" t="s">
+        <v>232</v>
       </c>
       <c r="B35" s="6" t="s">
         <v>129</v>
@@ -2606,8 +2991,8 @@
       </c>
     </row>
     <row r="36" spans="1:8" s="2" customFormat="1" ht="33" x14ac:dyDescent="0.3">
-      <c r="A36" s="7">
-        <v>35</v>
+      <c r="A36" s="7" t="s">
+        <v>233</v>
       </c>
       <c r="B36" s="6" t="s">
         <v>129</v>
@@ -2630,8 +3015,8 @@
       </c>
     </row>
     <row r="37" spans="1:8" s="10" customFormat="1" ht="82.5" x14ac:dyDescent="0.3">
-      <c r="A37" s="9">
-        <v>36</v>
+      <c r="A37" s="9" t="s">
+        <v>234</v>
       </c>
       <c r="B37" s="8" t="s">
         <v>129</v>
@@ -2656,8 +3041,8 @@
       </c>
     </row>
     <row r="38" spans="1:8" s="10" customFormat="1" ht="115.5" x14ac:dyDescent="0.3">
-      <c r="A38" s="9">
-        <v>37</v>
+      <c r="A38" s="9" t="s">
+        <v>235</v>
       </c>
       <c r="B38" s="8" t="s">
         <v>129</v>
@@ -2682,8 +3067,8 @@
       </c>
     </row>
     <row r="39" spans="1:8" s="10" customFormat="1" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="A39" s="9">
-        <v>38</v>
+      <c r="A39" s="9" t="s">
+        <v>236</v>
       </c>
       <c r="B39" s="8" t="s">
         <v>129</v>
@@ -2708,8 +3093,8 @@
       </c>
     </row>
     <row r="40" spans="1:8" s="10" customFormat="1" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="A40" s="9">
-        <v>39</v>
+      <c r="A40" s="9" t="s">
+        <v>237</v>
       </c>
       <c r="B40" s="8" t="s">
         <v>129</v>
@@ -2734,8 +3119,8 @@
       </c>
     </row>
     <row r="41" spans="1:8" s="10" customFormat="1" ht="66" x14ac:dyDescent="0.3">
-      <c r="A41" s="9">
-        <v>40</v>
+      <c r="A41" s="9" t="s">
+        <v>238</v>
       </c>
       <c r="B41" s="8" t="s">
         <v>129</v>
@@ -2760,8 +3145,8 @@
       </c>
     </row>
     <row r="42" spans="1:8" s="2" customFormat="1" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="A42" s="7">
-        <v>41</v>
+      <c r="A42" s="7" t="s">
+        <v>239</v>
       </c>
       <c r="B42" s="6" t="s">
         <v>129</v>
@@ -2784,8 +3169,8 @@
       <c r="H42" s="7"/>
     </row>
     <row r="43" spans="1:8" s="10" customFormat="1" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="A43" s="9">
-        <v>42</v>
+      <c r="A43" s="9" t="s">
+        <v>240</v>
       </c>
       <c r="B43" s="8" t="s">
         <v>129</v>
@@ -2810,8 +3195,8 @@
       </c>
     </row>
     <row r="44" spans="1:8" s="10" customFormat="1" ht="33" x14ac:dyDescent="0.3">
-      <c r="A44" s="9">
-        <v>43</v>
+      <c r="A44" s="9" t="s">
+        <v>241</v>
       </c>
       <c r="B44" s="8" t="s">
         <v>129</v>
@@ -2836,8 +3221,8 @@
       </c>
     </row>
     <row r="45" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="7">
-        <v>44</v>
+      <c r="A45" s="7" t="s">
+        <v>242</v>
       </c>
       <c r="B45" s="6" t="s">
         <v>129</v>
@@ -2862,8 +3247,8 @@
       </c>
     </row>
     <row r="46" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="7">
-        <v>45</v>
+      <c r="A46" s="7" t="s">
+        <v>243</v>
       </c>
       <c r="B46" s="6" t="s">
         <v>129</v>
@@ -2886,8 +3271,8 @@
       </c>
     </row>
     <row r="47" spans="1:8" s="2" customFormat="1" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="A47" s="7">
-        <v>46</v>
+      <c r="A47" s="7" t="s">
+        <v>244</v>
       </c>
       <c r="B47" s="6" t="s">
         <v>129</v>
@@ -2912,8 +3297,8 @@
       </c>
     </row>
     <row r="48" spans="1:8" s="10" customFormat="1" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="A48" s="9">
-        <v>47</v>
+      <c r="A48" s="9" t="s">
+        <v>245</v>
       </c>
       <c r="B48" s="8" t="s">
         <v>129</v>
@@ -2938,8 +3323,8 @@
       </c>
     </row>
     <row r="49" spans="1:8" s="2" customFormat="1" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="A49" s="7">
-        <v>48</v>
+      <c r="A49" s="7" t="s">
+        <v>246</v>
       </c>
       <c r="B49" s="6" t="s">
         <v>129</v>
@@ -2964,8 +3349,8 @@
       </c>
     </row>
     <row r="50" spans="1:8" s="2" customFormat="1" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="A50" s="7">
-        <v>49</v>
+      <c r="A50" s="7" t="s">
+        <v>247</v>
       </c>
       <c r="B50" s="6" t="s">
         <v>129</v>
@@ -2988,8 +3373,8 @@
       <c r="H50" s="7"/>
     </row>
     <row r="51" spans="1:8" s="10" customFormat="1" ht="33" x14ac:dyDescent="0.3">
-      <c r="A51" s="9">
-        <v>50</v>
+      <c r="A51" s="9" t="s">
+        <v>248</v>
       </c>
       <c r="B51" s="8" t="s">
         <v>129</v>
@@ -3014,8 +3399,8 @@
       </c>
     </row>
     <row r="52" spans="1:8" s="10" customFormat="1" ht="33" x14ac:dyDescent="0.3">
-      <c r="A52" s="9">
-        <v>51</v>
+      <c r="A52" s="9" t="s">
+        <v>249</v>
       </c>
       <c r="B52" s="8" t="s">
         <v>129</v>
@@ -3040,8 +3425,8 @@
       </c>
     </row>
     <row r="53" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="7">
-        <v>52</v>
+      <c r="A53" s="7" t="s">
+        <v>250</v>
       </c>
       <c r="B53" s="6" t="s">
         <v>129</v>
@@ -3064,8 +3449,8 @@
       </c>
     </row>
     <row r="54" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="7">
-        <v>53</v>
+      <c r="A54" s="7" t="s">
+        <v>251</v>
       </c>
       <c r="B54" s="6" t="s">
         <v>129</v>
@@ -3088,8 +3473,8 @@
       </c>
     </row>
     <row r="55" spans="1:8" s="10" customFormat="1" ht="99" x14ac:dyDescent="0.3">
-      <c r="A55" s="9">
-        <v>54</v>
+      <c r="A55" s="9" t="s">
+        <v>252</v>
       </c>
       <c r="B55" s="8" t="s">
         <v>129</v>
@@ -3114,8 +3499,8 @@
       </c>
     </row>
     <row r="56" spans="1:8" s="10" customFormat="1" ht="99" x14ac:dyDescent="0.3">
-      <c r="A56" s="15">
-        <v>55</v>
+      <c r="A56" s="9" t="s">
+        <v>253</v>
       </c>
       <c r="B56" s="14" t="s">
         <v>129</v>
@@ -3150,8 +3535,8 @@
       <c r="H57" s="18"/>
     </row>
     <row r="58" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="16">
-        <v>56</v>
+      <c r="A58" s="16" t="s">
+        <v>254</v>
       </c>
       <c r="B58" s="17" t="s">
         <v>135</v>
@@ -3172,8 +3557,8 @@
       <c r="H58" s="16"/>
     </row>
     <row r="59" spans="1:8" s="2" customFormat="1" ht="33" x14ac:dyDescent="0.3">
-      <c r="A59" s="7">
-        <v>57</v>
+      <c r="A59" s="7" t="s">
+        <v>255</v>
       </c>
       <c r="B59" s="6" t="s">
         <v>135</v>
@@ -3194,8 +3579,8 @@
       <c r="H59" s="7"/>
     </row>
     <row r="60" spans="1:8" s="10" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A60" s="9">
-        <v>58</v>
+      <c r="A60" s="9" t="s">
+        <v>256</v>
       </c>
       <c r="B60" s="8" t="s">
         <v>135</v>
@@ -3220,8 +3605,8 @@
       </c>
     </row>
     <row r="61" spans="1:8" s="2" customFormat="1" ht="33" x14ac:dyDescent="0.3">
-      <c r="A61" s="7">
-        <v>59</v>
+      <c r="A61" s="7" t="s">
+        <v>257</v>
       </c>
       <c r="B61" s="6" t="s">
         <v>135</v>
@@ -3242,8 +3627,8 @@
       <c r="H61" s="7"/>
     </row>
     <row r="63" spans="1:8" s="2" customFormat="1" ht="33" x14ac:dyDescent="0.3">
-      <c r="A63" s="7">
-        <v>60</v>
+      <c r="A63" s="7" t="s">
+        <v>258</v>
       </c>
       <c r="B63" s="6" t="s">
         <v>149</v>
@@ -3274,13 +3659,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6" customWidth="1"/>
     <col min="2" max="2" width="13.75" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="21.875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="36.125" customWidth="1"/>
@@ -3329,20 +3714,20 @@
       </c>
     </row>
     <row r="2" spans="1:11" s="3" customFormat="1" ht="33" x14ac:dyDescent="0.3">
-      <c r="A2" s="7">
-        <v>1</v>
+      <c r="A2" s="7" t="s">
+        <v>199</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>129</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>8</v>
+        <v>166</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>29</v>
+        <v>165</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>38</v>
+        <v>164</v>
       </c>
       <c r="F2" s="7" t="s">
         <v>105</v>
@@ -3358,17 +3743,17 @@
       </c>
     </row>
     <row r="3" spans="1:11" s="2" customFormat="1" ht="33" x14ac:dyDescent="0.3">
-      <c r="A3" s="7">
-        <v>2</v>
+      <c r="A3" s="7" t="s">
+        <v>200</v>
       </c>
       <c r="B3" s="7" t="s">
         <v>129</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>13</v>
+        <v>167</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>29</v>
+        <v>165</v>
       </c>
       <c r="E3" s="7" t="s">
         <v>40</v>
@@ -3387,20 +3772,20 @@
       </c>
     </row>
     <row r="4" spans="1:11" s="2" customFormat="1" ht="33" x14ac:dyDescent="0.3">
-      <c r="A4" s="7">
-        <v>3</v>
+      <c r="A4" s="7" t="s">
+        <v>201</v>
       </c>
       <c r="B4" s="7" t="s">
         <v>129</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>14</v>
+        <v>169</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>29</v>
+        <v>165</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>41</v>
+        <v>168</v>
       </c>
       <c r="F4" s="7" t="s">
         <v>105</v>
@@ -3416,20 +3801,20 @@
       </c>
     </row>
     <row r="5" spans="1:11" s="2" customFormat="1" ht="33" x14ac:dyDescent="0.3">
-      <c r="A5" s="7">
-        <v>4</v>
+      <c r="A5" s="7" t="s">
+        <v>202</v>
       </c>
       <c r="B5" s="7" t="s">
         <v>129</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>14</v>
+        <v>172</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>30</v>
+        <v>170</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>51</v>
+        <v>171</v>
       </c>
       <c r="F5" s="7" t="s">
         <v>104</v>
@@ -3445,17 +3830,17 @@
       </c>
     </row>
     <row r="6" spans="1:11" s="2" customFormat="1" ht="33" x14ac:dyDescent="0.3">
-      <c r="A6" s="7">
-        <v>5</v>
+      <c r="A6" s="7" t="s">
+        <v>203</v>
       </c>
       <c r="B6" s="7" t="s">
         <v>129</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>13</v>
+        <v>167</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>30</v>
+        <v>170</v>
       </c>
       <c r="E6" s="7" t="s">
         <v>111</v>
@@ -3474,20 +3859,20 @@
       </c>
     </row>
     <row r="7" spans="1:11" s="2" customFormat="1" ht="33" x14ac:dyDescent="0.3">
-      <c r="A7" s="7">
-        <v>6</v>
+      <c r="A7" s="7" t="s">
+        <v>204</v>
       </c>
       <c r="B7" s="7" t="s">
         <v>129</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>11</v>
+        <v>173</v>
       </c>
       <c r="D7" s="6" t="s">
         <v>30</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>42</v>
+        <v>174</v>
       </c>
       <c r="F7" s="7" t="s">
         <v>118</v>
@@ -3503,20 +3888,20 @@
       </c>
     </row>
     <row r="8" spans="1:11" s="2" customFormat="1" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="A8" s="7">
-        <v>7</v>
+      <c r="A8" s="7" t="s">
+        <v>205</v>
       </c>
       <c r="B8" s="7" t="s">
         <v>129</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>8</v>
+        <v>175</v>
       </c>
       <c r="D8" s="6" t="s">
         <v>44</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>43</v>
+        <v>176</v>
       </c>
       <c r="F8" s="7" t="s">
         <v>110</v>
@@ -3532,20 +3917,20 @@
       </c>
     </row>
     <row r="9" spans="1:11" s="2" customFormat="1" ht="33" x14ac:dyDescent="0.3">
-      <c r="A9" s="7">
-        <v>8</v>
+      <c r="A9" s="7" t="s">
+        <v>206</v>
       </c>
       <c r="B9" s="7" t="s">
         <v>129</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>8</v>
+        <v>177</v>
       </c>
       <c r="D9" s="6" t="s">
         <v>30</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>45</v>
+        <v>178</v>
       </c>
       <c r="F9" s="7" t="s">
         <v>104</v>
@@ -3561,20 +3946,20 @@
       </c>
     </row>
     <row r="10" spans="1:11" s="2" customFormat="1" ht="33" x14ac:dyDescent="0.3">
-      <c r="A10" s="7">
-        <v>10</v>
+      <c r="A10" s="7" t="s">
+        <v>259</v>
       </c>
       <c r="B10" s="7" t="s">
         <v>129</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>6</v>
+        <v>179</v>
       </c>
       <c r="D10" s="6" t="s">
         <v>30</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>49</v>
+        <v>180</v>
       </c>
       <c r="F10" s="7" t="s">
         <v>160</v>
@@ -3590,14 +3975,14 @@
       </c>
     </row>
     <row r="11" spans="1:11" s="2" customFormat="1" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="A11" s="7">
-        <v>13</v>
+      <c r="A11" s="7" t="s">
+        <v>260</v>
       </c>
       <c r="B11" s="7" t="s">
         <v>129</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>3</v>
+        <v>181</v>
       </c>
       <c r="D11" s="6" t="s">
         <v>30</v>
@@ -3619,20 +4004,20 @@
       </c>
     </row>
     <row r="12" spans="1:11" s="2" customFormat="1" ht="33" x14ac:dyDescent="0.3">
-      <c r="A12" s="7">
-        <v>29</v>
+      <c r="A12" s="7" t="s">
+        <v>261</v>
       </c>
       <c r="B12" s="6" t="s">
         <v>129</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>6</v>
+        <v>179</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>4</v>
+        <v>182</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>67</v>
+        <v>183</v>
       </c>
       <c r="F12" s="7" t="s">
         <v>116</v>
@@ -3648,20 +4033,20 @@
       </c>
     </row>
     <row r="13" spans="1:11" s="2" customFormat="1" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="A13" s="7">
-        <v>34</v>
+      <c r="A13" s="7" t="s">
+        <v>262</v>
       </c>
       <c r="B13" s="6" t="s">
         <v>129</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>6</v>
+        <v>179</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>31</v>
+        <v>184</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>70</v>
+        <v>185</v>
       </c>
       <c r="F13" s="7" t="s">
         <v>114</v>
@@ -3677,20 +4062,20 @@
       </c>
     </row>
     <row r="14" spans="1:11" s="2" customFormat="1" ht="33" x14ac:dyDescent="0.3">
-      <c r="A14" s="7">
-        <v>35</v>
+      <c r="A14" s="7" t="s">
+        <v>263</v>
       </c>
       <c r="B14" s="6" t="s">
         <v>129</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>8</v>
+        <v>166</v>
       </c>
       <c r="D14" s="6" t="s">
         <v>31</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>72</v>
+        <v>186</v>
       </c>
       <c r="F14" s="7" t="s">
         <v>115</v>
@@ -3704,17 +4089,17 @@
       </c>
     </row>
     <row r="15" spans="1:11" s="2" customFormat="1" ht="33" x14ac:dyDescent="0.3">
-      <c r="A15" s="7">
-        <v>41</v>
+      <c r="A15" s="7" t="s">
+        <v>264</v>
       </c>
       <c r="B15" s="6" t="s">
         <v>129</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>14</v>
+        <v>169</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>31</v>
+        <v>184</v>
       </c>
       <c r="E15" s="7" t="s">
         <v>76</v>
@@ -3731,8 +4116,8 @@
       <c r="K15" s="7"/>
     </row>
     <row r="16" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="7">
-        <v>44</v>
+      <c r="A16" s="7" t="s">
+        <v>265</v>
       </c>
       <c r="B16" s="6" t="s">
         <v>129</v>
@@ -3741,7 +4126,7 @@
         <v>14</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>33</v>
+        <v>187</v>
       </c>
       <c r="E16" s="7" t="s">
         <v>80</v>
@@ -3760,8 +4145,8 @@
       </c>
     </row>
     <row r="17" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="7">
-        <v>45</v>
+      <c r="A17" s="7" t="s">
+        <v>266</v>
       </c>
       <c r="B17" s="6" t="s">
         <v>129</v>
@@ -3773,7 +4158,7 @@
         <v>33</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>82</v>
+        <v>188</v>
       </c>
       <c r="F17" s="7" t="s">
         <v>118</v>
@@ -3787,20 +4172,20 @@
       </c>
     </row>
     <row r="18" spans="1:11" s="2" customFormat="1" ht="33" x14ac:dyDescent="0.3">
-      <c r="A18" s="7">
-        <v>46</v>
+      <c r="A18" s="7" t="s">
+        <v>267</v>
       </c>
       <c r="B18" s="6" t="s">
         <v>129</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>13</v>
+        <v>189</v>
       </c>
       <c r="D18" s="6" t="s">
         <v>33</v>
       </c>
       <c r="E18" s="7" t="s">
-        <v>83</v>
+        <v>190</v>
       </c>
       <c r="F18" s="7" t="s">
         <v>123</v>
@@ -3816,20 +4201,20 @@
       </c>
     </row>
     <row r="19" spans="1:11" s="2" customFormat="1" ht="33" x14ac:dyDescent="0.3">
-      <c r="A19" s="7">
-        <v>48</v>
+      <c r="A19" s="7" t="s">
+        <v>268</v>
       </c>
       <c r="B19" s="6" t="s">
         <v>129</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>8</v>
+        <v>166</v>
       </c>
       <c r="D19" s="6" t="s">
         <v>33</v>
       </c>
       <c r="E19" s="7" t="s">
-        <v>85</v>
+        <v>191</v>
       </c>
       <c r="F19" s="7" t="s">
         <v>126</v>
@@ -3845,14 +4230,14 @@
       </c>
     </row>
     <row r="20" spans="1:11" s="2" customFormat="1" ht="33" x14ac:dyDescent="0.3">
-      <c r="A20" s="7">
-        <v>49</v>
+      <c r="A20" s="7" t="s">
+        <v>269</v>
       </c>
       <c r="B20" s="6" t="s">
         <v>129</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>6</v>
+        <v>192</v>
       </c>
       <c r="D20" s="6" t="s">
         <v>33</v>
@@ -3872,14 +4257,14 @@
       <c r="K20" s="7"/>
     </row>
     <row r="21" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="7">
-        <v>52</v>
+      <c r="A21" s="7" t="s">
+        <v>270</v>
       </c>
       <c r="B21" s="6" t="s">
         <v>129</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>3</v>
+        <v>181</v>
       </c>
       <c r="D21" s="6" t="s">
         <v>33</v>
@@ -3899,8 +4284,8 @@
       </c>
     </row>
     <row r="22" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="7">
-        <v>53</v>
+      <c r="A22" s="7" t="s">
+        <v>271</v>
       </c>
       <c r="B22" s="6" t="s">
         <v>129</v>
@@ -3926,20 +4311,20 @@
       </c>
     </row>
     <row r="23" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="16">
-        <v>56</v>
+      <c r="A23" s="16" t="s">
+        <v>254</v>
       </c>
       <c r="B23" s="17" t="s">
         <v>135</v>
       </c>
       <c r="C23" s="17" t="s">
-        <v>136</v>
+        <v>193</v>
       </c>
       <c r="D23" s="17" t="s">
         <v>140</v>
       </c>
       <c r="E23" s="16" t="s">
-        <v>131</v>
+        <v>194</v>
       </c>
       <c r="F23" s="16" t="s">
         <v>143</v>
@@ -3951,14 +4336,14 @@
       <c r="K23" s="16"/>
     </row>
     <row r="24" spans="1:11" s="2" customFormat="1" ht="33" x14ac:dyDescent="0.3">
-      <c r="A24" s="7">
-        <v>57</v>
+      <c r="A24" s="7" t="s">
+        <v>255</v>
       </c>
       <c r="B24" s="6" t="s">
         <v>135</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>137</v>
+        <v>195</v>
       </c>
       <c r="D24" s="6" t="s">
         <v>141</v>
@@ -3976,8 +4361,8 @@
       <c r="K24" s="7"/>
     </row>
     <row r="25" spans="1:11" s="2" customFormat="1" ht="33" x14ac:dyDescent="0.3">
-      <c r="A25" s="7">
-        <v>59</v>
+      <c r="A25" s="7" t="s">
+        <v>272</v>
       </c>
       <c r="B25" s="6" t="s">
         <v>135</v>
@@ -3989,7 +4374,7 @@
         <v>139</v>
       </c>
       <c r="E25" s="7" t="s">
-        <v>134</v>
+        <v>196</v>
       </c>
       <c r="F25" s="7" t="s">
         <v>146</v>
@@ -4001,8 +4386,8 @@
       <c r="K25" s="7"/>
     </row>
     <row r="26" spans="1:11" s="2" customFormat="1" ht="33" x14ac:dyDescent="0.3">
-      <c r="A26" s="7">
-        <v>60</v>
+      <c r="A26" s="7" t="s">
+        <v>258</v>
       </c>
       <c r="B26" s="6" t="s">
         <v>149</v>
@@ -4011,10 +4396,10 @@
         <v>102</v>
       </c>
       <c r="D26" s="6" t="s">
-        <v>150</v>
+        <v>197</v>
       </c>
       <c r="E26" s="7" t="s">
-        <v>147</v>
+        <v>198</v>
       </c>
       <c r="F26" s="7" t="s">
         <v>148</v>

</xml_diff>

<commit_message>
[docs] update secure requirement and mitigation
update secure requirement and mitigation in threat_modeling file
</commit_message>
<xml_diff>
--- a/docs/05_threat_modeling/threat_modeling.xlsx
+++ b/docs/05_threat_modeling/threat_modeling.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\study\security\cmu\temp\cmu_project\docs\05_threat_modeling\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git-dir\cmu_project\docs\05_threat_modeling\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12390"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12390" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="threat_modeling_all" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="662" uniqueCount="273">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="676" uniqueCount="288">
   <si>
     <t>Id</t>
   </si>
@@ -602,48 +602,10 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>User Credential Data should be encrypted in the storage.</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>The login shall be authenticated in two ways.</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>the system shall know the change of the user credential data.</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>the system shall know the change of the user credential data.</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>클라이언트와 서버는 상호인증을 해야 한다.</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>서버와 클라이언트는 암호화된 채널을 통하여 통신하여야 한다.</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>Need to use TLS</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>using TLS</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>모든 입력은 사용하기 전에 검증하여야 한다.
-need input sanitization</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">
-The number of images should be under 100.</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t xml:space="preserve">If the user credential data is stored as plain text, it can be disclosed. </t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -660,10 +622,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>An attacker modify user credential data and then server can use it without checking.</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>Spoofing</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -1026,13 +984,159 @@
   </si>
   <si>
     <t>TR-59</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>User Credential Data should be encrypted in the storage.
+Use well-known cryptographic libraries and robust algorithms.</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Encrypt user credential data in storage
+- Use OpenSSL library of latest version (1.1.1k)
+- Use an algorithm that are stronger than AES256
+- Use cbc of gcm mode
+Integrity Check with hash (optional when using cbc mode)
+- Use an alforithm that are stronger than sha256</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>the system shall know the change of the user credential data.
+The system must perform an integrity check before using user credentials.
+Use well-known cryptographic libraries and robust algorithms.</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Integrity Check with hash functionan
+- Use OpenSSL library of latest version (1.1.1k)
+- Use an algorithm that are stronger than sha256
+Encrypt User credential (optional)
+- Use an algorithm that are stronger than AES256
+- Use cbc of gcm mode</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Apply setting policy of cryptographically strong password
+- Enforce passwords longer than 10(?) characters.
+- Forces the use of mixed uppercase and lowercase letters of the alphabet
+Strong authentication method
+- Condider 2-Factor-Authentication method</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Cryptographically strong password should be used.
+A strong authentication method should be used.</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Server and client must communicate using an encrypted channel.</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Input validation check
+- Input sanitization
+Integrity Check with hash functionan
+- Use OpenSSL library of latest version (1.1.1k)
+- Use an algorithm that are stronger than sha256
+Communicate using Encryted channel
+- using protocol TLS1.2 or higher
+- Consider mutual authentication between server and client</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Communicate using Encryted channel
+- using protocol TLS1.2 or higher
+- Consider mutual authentication between server and client</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Only the verified server and client should be connected and communicated.
+Save contents of the communication as a log and use as proof of non-repudiation.</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Use mutual authentification
+- Using protocol TLS1.2 or higher
+- Use mutual authentication between server and client
+Save contents of communication as a log
+- Save log of the request and response between the server and the client</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Server and client must communicate using an encrypted channel.</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Cryptographically strong password should be used.
+A strong authentication method should be used.</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Server and client must communicate using an encrypted channel.
+Only the verified server and client should be connected and communicated.</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Communicate using Encryted channel
+- using protocol TLS1.2 or higher
+- Consider mutual authentication between server and client</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>the system shall know the change of the user credential data.
+Server and client must communicate using an encrypted channel.
+Input validation check is required in Server side.</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Input validation check is required in Server side.</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Input validation check
+- Input sanitization</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Protect Camera from physical damage</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Protect from physical damage
+- Wrap the camera module out of sight, or glue the cable to the camera.</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Restrictions related to files are necessary to avoid system problems.</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Validation of image when file saving
+- Limit on number of files
+- File name verification when image save
+- File size validation when image save</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Errors, exceptions, and abnormal conditions that may occur in the software must be handled robustly.</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Implement robust system
+- Error handling
+- Exception handling
+- Finding countermeasures for predictable abnormal conditions</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Input validation check is required in Client side.</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -2081,7 +2185,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H63"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
     </sheetView>
@@ -2126,7 +2230,7 @@
     </row>
     <row r="2" spans="1:8" s="3" customFormat="1" ht="33" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
-        <v>199</v>
+        <v>189</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>129</v>
@@ -2150,7 +2254,7 @@
     </row>
     <row r="3" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
-        <v>200</v>
+        <v>190</v>
       </c>
       <c r="B3" s="7" t="s">
         <v>129</v>
@@ -2174,7 +2278,7 @@
     </row>
     <row r="4" spans="1:8" s="2" customFormat="1" ht="33" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
-        <v>201</v>
+        <v>191</v>
       </c>
       <c r="B4" s="7" t="s">
         <v>129</v>
@@ -2198,7 +2302,7 @@
     </row>
     <row r="5" spans="1:8" s="2" customFormat="1" ht="33" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
-        <v>202</v>
+        <v>192</v>
       </c>
       <c r="B5" s="7" t="s">
         <v>129</v>
@@ -2222,7 +2326,7 @@
     </row>
     <row r="6" spans="1:8" s="2" customFormat="1" ht="33" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
-        <v>203</v>
+        <v>193</v>
       </c>
       <c r="B6" s="7" t="s">
         <v>129</v>
@@ -2246,7 +2350,7 @@
     </row>
     <row r="7" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
-        <v>204</v>
+        <v>194</v>
       </c>
       <c r="B7" s="7" t="s">
         <v>129</v>
@@ -2270,7 +2374,7 @@
     </row>
     <row r="8" spans="1:8" s="2" customFormat="1" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
-        <v>205</v>
+        <v>195</v>
       </c>
       <c r="B8" s="7" t="s">
         <v>129</v>
@@ -2294,7 +2398,7 @@
     </row>
     <row r="9" spans="1:8" s="2" customFormat="1" ht="33" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
-        <v>206</v>
+        <v>196</v>
       </c>
       <c r="B9" s="7" t="s">
         <v>129</v>
@@ -2318,7 +2422,7 @@
     </row>
     <row r="10" spans="1:8" s="10" customFormat="1" ht="33" x14ac:dyDescent="0.3">
       <c r="A10" s="9" t="s">
-        <v>207</v>
+        <v>197</v>
       </c>
       <c r="B10" s="8" t="s">
         <v>129</v>
@@ -2344,7 +2448,7 @@
     </row>
     <row r="11" spans="1:8" s="2" customFormat="1" ht="33" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
-        <v>208</v>
+        <v>198</v>
       </c>
       <c r="B11" s="7" t="s">
         <v>129</v>
@@ -2368,7 +2472,7 @@
     </row>
     <row r="12" spans="1:8" s="10" customFormat="1" ht="33" x14ac:dyDescent="0.3">
       <c r="A12" s="9" t="s">
-        <v>209</v>
+        <v>199</v>
       </c>
       <c r="B12" s="8" t="s">
         <v>129</v>
@@ -2394,7 +2498,7 @@
     </row>
     <row r="13" spans="1:8" s="10" customFormat="1" ht="33" x14ac:dyDescent="0.3">
       <c r="A13" s="9" t="s">
-        <v>210</v>
+        <v>200</v>
       </c>
       <c r="B13" s="8" t="s">
         <v>129</v>
@@ -2420,7 +2524,7 @@
     </row>
     <row r="14" spans="1:8" s="2" customFormat="1" ht="33" x14ac:dyDescent="0.3">
       <c r="A14" s="7" t="s">
-        <v>211</v>
+        <v>201</v>
       </c>
       <c r="B14" s="7" t="s">
         <v>129</v>
@@ -2446,7 +2550,7 @@
     </row>
     <row r="15" spans="1:8" s="10" customFormat="1" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A15" s="9" t="s">
-        <v>212</v>
+        <v>202</v>
       </c>
       <c r="B15" s="8" t="s">
         <v>129</v>
@@ -2472,7 +2576,7 @@
     </row>
     <row r="16" spans="1:8" s="10" customFormat="1" ht="33" x14ac:dyDescent="0.3">
       <c r="A16" s="9" t="s">
-        <v>213</v>
+        <v>203</v>
       </c>
       <c r="B16" s="8" t="s">
         <v>129</v>
@@ -2498,7 +2602,7 @@
     </row>
     <row r="17" spans="1:8" s="10" customFormat="1" ht="66" x14ac:dyDescent="0.3">
       <c r="A17" s="9" t="s">
-        <v>214</v>
+        <v>204</v>
       </c>
       <c r="B17" s="8" t="s">
         <v>129</v>
@@ -2524,7 +2628,7 @@
     </row>
     <row r="18" spans="1:8" s="10" customFormat="1" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A18" s="9" t="s">
-        <v>215</v>
+        <v>205</v>
       </c>
       <c r="B18" s="8" t="s">
         <v>129</v>
@@ -2550,7 +2654,7 @@
     </row>
     <row r="19" spans="1:8" s="10" customFormat="1" ht="82.5" x14ac:dyDescent="0.3">
       <c r="A19" s="9" t="s">
-        <v>216</v>
+        <v>206</v>
       </c>
       <c r="B19" s="8" t="s">
         <v>129</v>
@@ -2576,7 +2680,7 @@
     </row>
     <row r="20" spans="1:8" s="10" customFormat="1" ht="33" x14ac:dyDescent="0.3">
       <c r="A20" s="9" t="s">
-        <v>217</v>
+        <v>207</v>
       </c>
       <c r="B20" s="8" t="s">
         <v>129</v>
@@ -2602,7 +2706,7 @@
     </row>
     <row r="21" spans="1:8" s="10" customFormat="1" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A21" s="9" t="s">
-        <v>218</v>
+        <v>208</v>
       </c>
       <c r="B21" s="8" t="s">
         <v>129</v>
@@ -2628,7 +2732,7 @@
     </row>
     <row r="22" spans="1:8" s="10" customFormat="1" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A22" s="9" t="s">
-        <v>219</v>
+        <v>209</v>
       </c>
       <c r="B22" s="8" t="s">
         <v>129</v>
@@ -2654,7 +2758,7 @@
     </row>
     <row r="23" spans="1:8" s="10" customFormat="1" ht="33" x14ac:dyDescent="0.3">
       <c r="A23" s="9" t="s">
-        <v>220</v>
+        <v>210</v>
       </c>
       <c r="B23" s="8" t="s">
         <v>129</v>
@@ -2680,7 +2784,7 @@
     </row>
     <row r="24" spans="1:8" s="10" customFormat="1" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A24" s="9" t="s">
-        <v>221</v>
+        <v>211</v>
       </c>
       <c r="B24" s="8" t="s">
         <v>129</v>
@@ -2706,7 +2810,7 @@
     </row>
     <row r="25" spans="1:8" s="10" customFormat="1" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A25" s="9" t="s">
-        <v>222</v>
+        <v>212</v>
       </c>
       <c r="B25" s="8" t="s">
         <v>129</v>
@@ -2732,7 +2836,7 @@
     </row>
     <row r="26" spans="1:8" s="10" customFormat="1" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A26" s="9" t="s">
-        <v>223</v>
+        <v>213</v>
       </c>
       <c r="B26" s="8" t="s">
         <v>129</v>
@@ -2758,7 +2862,7 @@
     </row>
     <row r="27" spans="1:8" s="10" customFormat="1" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A27" s="9" t="s">
-        <v>224</v>
+        <v>214</v>
       </c>
       <c r="B27" s="8" t="s">
         <v>129</v>
@@ -2784,7 +2888,7 @@
     </row>
     <row r="28" spans="1:8" s="10" customFormat="1" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A28" s="9" t="s">
-        <v>225</v>
+        <v>215</v>
       </c>
       <c r="B28" s="8" t="s">
         <v>129</v>
@@ -2810,7 +2914,7 @@
     </row>
     <row r="29" spans="1:8" s="10" customFormat="1" ht="82.5" x14ac:dyDescent="0.3">
       <c r="A29" s="9" t="s">
-        <v>226</v>
+        <v>216</v>
       </c>
       <c r="B29" s="8" t="s">
         <v>129</v>
@@ -2836,7 +2940,7 @@
     </row>
     <row r="30" spans="1:8" s="2" customFormat="1" ht="33" x14ac:dyDescent="0.3">
       <c r="A30" s="7" t="s">
-        <v>227</v>
+        <v>217</v>
       </c>
       <c r="B30" s="6" t="s">
         <v>129</v>
@@ -2862,7 +2966,7 @@
     </row>
     <row r="31" spans="1:8" s="10" customFormat="1" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A31" s="9" t="s">
-        <v>228</v>
+        <v>218</v>
       </c>
       <c r="B31" s="8" t="s">
         <v>129</v>
@@ -2888,7 +2992,7 @@
     </row>
     <row r="32" spans="1:8" s="10" customFormat="1" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A32" s="9" t="s">
-        <v>229</v>
+        <v>219</v>
       </c>
       <c r="B32" s="8" t="s">
         <v>129</v>
@@ -2914,7 +3018,7 @@
     </row>
     <row r="33" spans="1:8" s="10" customFormat="1" ht="33" x14ac:dyDescent="0.3">
       <c r="A33" s="9" t="s">
-        <v>230</v>
+        <v>220</v>
       </c>
       <c r="B33" s="8" t="s">
         <v>129</v>
@@ -2940,7 +3044,7 @@
     </row>
     <row r="34" spans="1:8" s="10" customFormat="1" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A34" s="9" t="s">
-        <v>231</v>
+        <v>221</v>
       </c>
       <c r="B34" s="8" t="s">
         <v>129</v>
@@ -2966,7 +3070,7 @@
     </row>
     <row r="35" spans="1:8" s="2" customFormat="1" ht="33" x14ac:dyDescent="0.3">
       <c r="A35" s="7" t="s">
-        <v>232</v>
+        <v>222</v>
       </c>
       <c r="B35" s="6" t="s">
         <v>129</v>
@@ -2992,7 +3096,7 @@
     </row>
     <row r="36" spans="1:8" s="2" customFormat="1" ht="33" x14ac:dyDescent="0.3">
       <c r="A36" s="7" t="s">
-        <v>233</v>
+        <v>223</v>
       </c>
       <c r="B36" s="6" t="s">
         <v>129</v>
@@ -3016,7 +3120,7 @@
     </row>
     <row r="37" spans="1:8" s="10" customFormat="1" ht="82.5" x14ac:dyDescent="0.3">
       <c r="A37" s="9" t="s">
-        <v>234</v>
+        <v>224</v>
       </c>
       <c r="B37" s="8" t="s">
         <v>129</v>
@@ -3042,7 +3146,7 @@
     </row>
     <row r="38" spans="1:8" s="10" customFormat="1" ht="115.5" x14ac:dyDescent="0.3">
       <c r="A38" s="9" t="s">
-        <v>235</v>
+        <v>225</v>
       </c>
       <c r="B38" s="8" t="s">
         <v>129</v>
@@ -3068,7 +3172,7 @@
     </row>
     <row r="39" spans="1:8" s="10" customFormat="1" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A39" s="9" t="s">
-        <v>236</v>
+        <v>226</v>
       </c>
       <c r="B39" s="8" t="s">
         <v>129</v>
@@ -3094,7 +3198,7 @@
     </row>
     <row r="40" spans="1:8" s="10" customFormat="1" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A40" s="9" t="s">
-        <v>237</v>
+        <v>227</v>
       </c>
       <c r="B40" s="8" t="s">
         <v>129</v>
@@ -3120,7 +3224,7 @@
     </row>
     <row r="41" spans="1:8" s="10" customFormat="1" ht="66" x14ac:dyDescent="0.3">
       <c r="A41" s="9" t="s">
-        <v>238</v>
+        <v>228</v>
       </c>
       <c r="B41" s="8" t="s">
         <v>129</v>
@@ -3146,7 +3250,7 @@
     </row>
     <row r="42" spans="1:8" s="2" customFormat="1" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A42" s="7" t="s">
-        <v>239</v>
+        <v>229</v>
       </c>
       <c r="B42" s="6" t="s">
         <v>129</v>
@@ -3170,7 +3274,7 @@
     </row>
     <row r="43" spans="1:8" s="10" customFormat="1" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A43" s="9" t="s">
-        <v>240</v>
+        <v>230</v>
       </c>
       <c r="B43" s="8" t="s">
         <v>129</v>
@@ -3196,7 +3300,7 @@
     </row>
     <row r="44" spans="1:8" s="10" customFormat="1" ht="33" x14ac:dyDescent="0.3">
       <c r="A44" s="9" t="s">
-        <v>241</v>
+        <v>231</v>
       </c>
       <c r="B44" s="8" t="s">
         <v>129</v>
@@ -3222,7 +3326,7 @@
     </row>
     <row r="45" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A45" s="7" t="s">
-        <v>242</v>
+        <v>232</v>
       </c>
       <c r="B45" s="6" t="s">
         <v>129</v>
@@ -3248,7 +3352,7 @@
     </row>
     <row r="46" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A46" s="7" t="s">
-        <v>243</v>
+        <v>233</v>
       </c>
       <c r="B46" s="6" t="s">
         <v>129</v>
@@ -3272,7 +3376,7 @@
     </row>
     <row r="47" spans="1:8" s="2" customFormat="1" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A47" s="7" t="s">
-        <v>244</v>
+        <v>234</v>
       </c>
       <c r="B47" s="6" t="s">
         <v>129</v>
@@ -3298,7 +3402,7 @@
     </row>
     <row r="48" spans="1:8" s="10" customFormat="1" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A48" s="9" t="s">
-        <v>245</v>
+        <v>235</v>
       </c>
       <c r="B48" s="8" t="s">
         <v>129</v>
@@ -3324,7 +3428,7 @@
     </row>
     <row r="49" spans="1:8" s="2" customFormat="1" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A49" s="7" t="s">
-        <v>246</v>
+        <v>236</v>
       </c>
       <c r="B49" s="6" t="s">
         <v>129</v>
@@ -3350,7 +3454,7 @@
     </row>
     <row r="50" spans="1:8" s="2" customFormat="1" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A50" s="7" t="s">
-        <v>247</v>
+        <v>237</v>
       </c>
       <c r="B50" s="6" t="s">
         <v>129</v>
@@ -3374,7 +3478,7 @@
     </row>
     <row r="51" spans="1:8" s="10" customFormat="1" ht="33" x14ac:dyDescent="0.3">
       <c r="A51" s="9" t="s">
-        <v>248</v>
+        <v>238</v>
       </c>
       <c r="B51" s="8" t="s">
         <v>129</v>
@@ -3400,7 +3504,7 @@
     </row>
     <row r="52" spans="1:8" s="10" customFormat="1" ht="33" x14ac:dyDescent="0.3">
       <c r="A52" s="9" t="s">
-        <v>249</v>
+        <v>239</v>
       </c>
       <c r="B52" s="8" t="s">
         <v>129</v>
@@ -3426,7 +3530,7 @@
     </row>
     <row r="53" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A53" s="7" t="s">
-        <v>250</v>
+        <v>240</v>
       </c>
       <c r="B53" s="6" t="s">
         <v>129</v>
@@ -3450,7 +3554,7 @@
     </row>
     <row r="54" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A54" s="7" t="s">
-        <v>251</v>
+        <v>241</v>
       </c>
       <c r="B54" s="6" t="s">
         <v>129</v>
@@ -3474,7 +3578,7 @@
     </row>
     <row r="55" spans="1:8" s="10" customFormat="1" ht="99" x14ac:dyDescent="0.3">
       <c r="A55" s="9" t="s">
-        <v>252</v>
+        <v>242</v>
       </c>
       <c r="B55" s="8" t="s">
         <v>129</v>
@@ -3500,7 +3604,7 @@
     </row>
     <row r="56" spans="1:8" s="10" customFormat="1" ht="99" x14ac:dyDescent="0.3">
       <c r="A56" s="9" t="s">
-        <v>253</v>
+        <v>243</v>
       </c>
       <c r="B56" s="14" t="s">
         <v>129</v>
@@ -3536,7 +3640,7 @@
     </row>
     <row r="58" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A58" s="16" t="s">
-        <v>254</v>
+        <v>244</v>
       </c>
       <c r="B58" s="17" t="s">
         <v>135</v>
@@ -3558,7 +3662,7 @@
     </row>
     <row r="59" spans="1:8" s="2" customFormat="1" ht="33" x14ac:dyDescent="0.3">
       <c r="A59" s="7" t="s">
-        <v>255</v>
+        <v>245</v>
       </c>
       <c r="B59" s="6" t="s">
         <v>135</v>
@@ -3580,7 +3684,7 @@
     </row>
     <row r="60" spans="1:8" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A60" s="9" t="s">
-        <v>256</v>
+        <v>246</v>
       </c>
       <c r="B60" s="8" t="s">
         <v>135</v>
@@ -3606,7 +3710,7 @@
     </row>
     <row r="61" spans="1:8" s="2" customFormat="1" ht="33" x14ac:dyDescent="0.3">
       <c r="A61" s="7" t="s">
-        <v>257</v>
+        <v>247</v>
       </c>
       <c r="B61" s="6" t="s">
         <v>135</v>
@@ -3628,7 +3732,7 @@
     </row>
     <row r="63" spans="1:8" s="2" customFormat="1" ht="33" x14ac:dyDescent="0.3">
       <c r="A63" s="7" t="s">
-        <v>258</v>
+        <v>248</v>
       </c>
       <c r="B63" s="6" t="s">
         <v>149</v>
@@ -3659,8 +3763,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K26"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView tabSelected="1" topLeftCell="B25" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F34" sqref="F34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -3713,21 +3817,21 @@
         <v>92</v>
       </c>
     </row>
-    <row r="2" spans="1:11" s="3" customFormat="1" ht="33" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" s="3" customFormat="1" ht="165" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
-        <v>199</v>
+        <v>189</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>129</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>166</v>
+        <v>157</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>165</v>
+        <v>156</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="F2" s="7" t="s">
         <v>105</v>
@@ -3736,24 +3840,24 @@
       <c r="H2" s="7"/>
       <c r="I2" s="7"/>
       <c r="J2" s="7" t="s">
-        <v>154</v>
+        <v>263</v>
       </c>
       <c r="K2" s="7" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" s="2" customFormat="1" ht="33" x14ac:dyDescent="0.3">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" s="2" customFormat="1" ht="148.5" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
-        <v>200</v>
+        <v>190</v>
       </c>
       <c r="B3" s="7" t="s">
         <v>129</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>167</v>
+        <v>158</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>165</v>
+        <v>156</v>
       </c>
       <c r="E3" s="7" t="s">
         <v>40</v>
@@ -3765,27 +3869,27 @@
       <c r="H3" s="7"/>
       <c r="I3" s="7"/>
       <c r="J3" s="7" t="s">
-        <v>157</v>
+        <v>265</v>
       </c>
       <c r="K3" s="7" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" s="2" customFormat="1" ht="33" x14ac:dyDescent="0.3">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" s="2" customFormat="1" ht="181.5" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
-        <v>201</v>
+        <v>191</v>
       </c>
       <c r="B4" s="7" t="s">
         <v>129</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>169</v>
+        <v>159</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>165</v>
+        <v>156</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>168</v>
+        <v>41</v>
       </c>
       <c r="F4" s="7" t="s">
         <v>105</v>
@@ -3794,27 +3898,27 @@
       <c r="H4" s="7"/>
       <c r="I4" s="7"/>
       <c r="J4" s="7" t="s">
-        <v>156</v>
+        <v>278</v>
       </c>
       <c r="K4" s="7" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" s="2" customFormat="1" ht="33" x14ac:dyDescent="0.3">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" s="2" customFormat="1" ht="148.5" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
-        <v>202</v>
+        <v>192</v>
       </c>
       <c r="B5" s="7" t="s">
         <v>129</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>172</v>
+        <v>162</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>170</v>
+        <v>160</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>171</v>
+        <v>161</v>
       </c>
       <c r="F5" s="7" t="s">
         <v>104</v>
@@ -3823,24 +3927,24 @@
       <c r="H5" s="7"/>
       <c r="I5" s="7"/>
       <c r="J5" s="7" t="s">
-        <v>155</v>
+        <v>268</v>
       </c>
       <c r="K5" s="7" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" s="2" customFormat="1" ht="33" x14ac:dyDescent="0.3">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" s="2" customFormat="1" ht="66" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
-        <v>203</v>
+        <v>193</v>
       </c>
       <c r="B6" s="7" t="s">
         <v>129</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>167</v>
+        <v>158</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>170</v>
+        <v>160</v>
       </c>
       <c r="E6" s="7" t="s">
         <v>111</v>
@@ -3852,27 +3956,27 @@
       <c r="H6" s="7"/>
       <c r="I6" s="7"/>
       <c r="J6" s="7" t="s">
-        <v>159</v>
+        <v>269</v>
       </c>
       <c r="K6" s="7" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" s="2" customFormat="1" ht="33" x14ac:dyDescent="0.3">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" s="2" customFormat="1" ht="132" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
-        <v>204</v>
+        <v>194</v>
       </c>
       <c r="B7" s="7" t="s">
         <v>129</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>173</v>
+        <v>163</v>
       </c>
       <c r="D7" s="6" t="s">
         <v>30</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>174</v>
+        <v>164</v>
       </c>
       <c r="F7" s="7" t="s">
         <v>118</v>
@@ -3881,27 +3985,27 @@
       <c r="H7" s="7"/>
       <c r="I7" s="7"/>
       <c r="J7" s="7" t="s">
-        <v>158</v>
+        <v>272</v>
       </c>
       <c r="K7" s="7" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" s="2" customFormat="1" ht="49.5" x14ac:dyDescent="0.3">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" s="2" customFormat="1" ht="66" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
-        <v>205</v>
+        <v>195</v>
       </c>
       <c r="B8" s="7" t="s">
         <v>129</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>175</v>
+        <v>165</v>
       </c>
       <c r="D8" s="6" t="s">
         <v>44</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>176</v>
+        <v>166</v>
       </c>
       <c r="F8" s="7" t="s">
         <v>110</v>
@@ -3910,27 +4014,27 @@
       <c r="H8" s="7"/>
       <c r="I8" s="7"/>
       <c r="J8" s="7" t="s">
-        <v>159</v>
+        <v>274</v>
       </c>
       <c r="K8" s="7" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" s="2" customFormat="1" ht="33" x14ac:dyDescent="0.3">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" s="2" customFormat="1" ht="148.5" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
-        <v>206</v>
+        <v>196</v>
       </c>
       <c r="B9" s="7" t="s">
         <v>129</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>177</v>
+        <v>167</v>
       </c>
       <c r="D9" s="6" t="s">
         <v>30</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>178</v>
+        <v>168</v>
       </c>
       <c r="F9" s="7" t="s">
         <v>104</v>
@@ -3939,50 +4043,50 @@
       <c r="H9" s="7"/>
       <c r="I9" s="7"/>
       <c r="J9" s="7" t="s">
-        <v>155</v>
+        <v>275</v>
       </c>
       <c r="K9" s="7" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" s="2" customFormat="1" ht="33" x14ac:dyDescent="0.3">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" s="2" customFormat="1" ht="82.5" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
-        <v>259</v>
+        <v>249</v>
       </c>
       <c r="B10" s="7" t="s">
         <v>129</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>179</v>
+        <v>169</v>
       </c>
       <c r="D10" s="6" t="s">
         <v>30</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>180</v>
+        <v>170</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="G10" s="7"/>
       <c r="H10" s="7"/>
       <c r="I10" s="7"/>
       <c r="J10" s="7" t="s">
-        <v>159</v>
+        <v>276</v>
       </c>
       <c r="K10" s="7" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" s="2" customFormat="1" ht="49.5" x14ac:dyDescent="0.3">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" s="2" customFormat="1" ht="33" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
-        <v>260</v>
+        <v>250</v>
       </c>
       <c r="B11" s="7" t="s">
         <v>129</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>181</v>
+        <v>171</v>
       </c>
       <c r="D11" s="6" t="s">
         <v>30</v>
@@ -3997,27 +4101,27 @@
       <c r="H11" s="7"/>
       <c r="I11" s="7"/>
       <c r="J11" s="7" t="s">
-        <v>162</v>
+        <v>279</v>
       </c>
       <c r="K11" s="7" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" s="2" customFormat="1" ht="33" x14ac:dyDescent="0.3">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" s="2" customFormat="1" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
-        <v>261</v>
+        <v>251</v>
       </c>
       <c r="B12" s="6" t="s">
         <v>129</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>179</v>
+        <v>169</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>182</v>
+        <v>172</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>183</v>
+        <v>173</v>
       </c>
       <c r="F12" s="7" t="s">
         <v>116</v>
@@ -4026,27 +4130,27 @@
       <c r="H12" s="7"/>
       <c r="I12" s="7"/>
       <c r="J12" s="7" t="s">
-        <v>117</v>
+        <v>281</v>
       </c>
       <c r="K12" s="7" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" s="2" customFormat="1" ht="49.5" x14ac:dyDescent="0.3">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" s="2" customFormat="1" ht="82.5" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
-        <v>262</v>
+        <v>252</v>
       </c>
       <c r="B13" s="6" t="s">
         <v>129</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>179</v>
+        <v>169</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>184</v>
+        <v>174</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>185</v>
+        <v>175</v>
       </c>
       <c r="F13" s="7" t="s">
         <v>114</v>
@@ -4055,27 +4159,27 @@
       <c r="H13" s="7"/>
       <c r="I13" s="7"/>
       <c r="J13" s="7" t="s">
-        <v>163</v>
+        <v>283</v>
       </c>
       <c r="K13" s="7" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" s="2" customFormat="1" ht="33" x14ac:dyDescent="0.3">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" s="2" customFormat="1" ht="165" x14ac:dyDescent="0.3">
       <c r="A14" s="7" t="s">
-        <v>263</v>
+        <v>253</v>
       </c>
       <c r="B14" s="6" t="s">
         <v>129</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>166</v>
+        <v>157</v>
       </c>
       <c r="D14" s="6" t="s">
         <v>31</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>186</v>
+        <v>176</v>
       </c>
       <c r="F14" s="7" t="s">
         <v>115</v>
@@ -4083,23 +4187,25 @@
       <c r="G14" s="7"/>
       <c r="H14" s="7"/>
       <c r="I14" s="7"/>
-      <c r="J14" s="7"/>
+      <c r="J14" s="7" t="s">
+        <v>263</v>
+      </c>
       <c r="K14" s="7" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" s="2" customFormat="1" ht="33" x14ac:dyDescent="0.3">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" s="2" customFormat="1" ht="165" x14ac:dyDescent="0.3">
       <c r="A15" s="7" t="s">
-        <v>264</v>
+        <v>254</v>
       </c>
       <c r="B15" s="6" t="s">
         <v>129</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>169</v>
+        <v>159</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>184</v>
+        <v>174</v>
       </c>
       <c r="E15" s="7" t="s">
         <v>76</v>
@@ -4111,13 +4217,15 @@
       <c r="H15" s="7"/>
       <c r="I15" s="7"/>
       <c r="J15" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="K15" s="7"/>
-    </row>
-    <row r="16" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.3">
+        <v>263</v>
+      </c>
+      <c r="K15" s="7" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" s="2" customFormat="1" ht="82.5" x14ac:dyDescent="0.3">
       <c r="A16" s="7" t="s">
-        <v>265</v>
+        <v>255</v>
       </c>
       <c r="B16" s="6" t="s">
         <v>129</v>
@@ -4126,7 +4234,7 @@
         <v>14</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
       <c r="E16" s="7" t="s">
         <v>80</v>
@@ -4138,15 +4246,15 @@
       <c r="H16" s="7"/>
       <c r="I16" s="7"/>
       <c r="J16" s="7" t="s">
-        <v>81</v>
+        <v>276</v>
       </c>
       <c r="K16" s="7" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.3">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" s="2" customFormat="1" ht="82.5" x14ac:dyDescent="0.3">
       <c r="A17" s="7" t="s">
-        <v>266</v>
+        <v>256</v>
       </c>
       <c r="B17" s="6" t="s">
         <v>129</v>
@@ -4158,7 +4266,7 @@
         <v>33</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>188</v>
+        <v>178</v>
       </c>
       <c r="F17" s="7" t="s">
         <v>118</v>
@@ -4166,26 +4274,28 @@
       <c r="G17" s="7"/>
       <c r="H17" s="7"/>
       <c r="I17" s="7"/>
-      <c r="J17" s="7"/>
+      <c r="J17" s="7" t="s">
+        <v>276</v>
+      </c>
       <c r="K17" s="7" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" s="2" customFormat="1" ht="33" x14ac:dyDescent="0.3">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" s="2" customFormat="1" ht="66" x14ac:dyDescent="0.3">
       <c r="A18" s="7" t="s">
-        <v>267</v>
+        <v>257</v>
       </c>
       <c r="B18" s="6" t="s">
         <v>129</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>189</v>
+        <v>179</v>
       </c>
       <c r="D18" s="6" t="s">
         <v>33</v>
       </c>
       <c r="E18" s="7" t="s">
-        <v>190</v>
+        <v>180</v>
       </c>
       <c r="F18" s="7" t="s">
         <v>123</v>
@@ -4197,24 +4307,24 @@
         <v>124</v>
       </c>
       <c r="K18" s="7" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" s="2" customFormat="1" ht="33" x14ac:dyDescent="0.3">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" s="2" customFormat="1" ht="66" x14ac:dyDescent="0.3">
       <c r="A19" s="7" t="s">
-        <v>268</v>
+        <v>258</v>
       </c>
       <c r="B19" s="6" t="s">
         <v>129</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>166</v>
+        <v>157</v>
       </c>
       <c r="D19" s="6" t="s">
         <v>33</v>
       </c>
       <c r="E19" s="7" t="s">
-        <v>191</v>
+        <v>181</v>
       </c>
       <c r="F19" s="7" t="s">
         <v>126</v>
@@ -4226,18 +4336,18 @@
         <v>124</v>
       </c>
       <c r="K19" s="7" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" s="2" customFormat="1" ht="33" x14ac:dyDescent="0.3">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" s="2" customFormat="1" ht="82.5" x14ac:dyDescent="0.3">
       <c r="A20" s="7" t="s">
-        <v>269</v>
+        <v>259</v>
       </c>
       <c r="B20" s="6" t="s">
         <v>129</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>192</v>
+        <v>182</v>
       </c>
       <c r="D20" s="6" t="s">
         <v>33</v>
@@ -4252,19 +4362,21 @@
       <c r="H20" s="7"/>
       <c r="I20" s="7"/>
       <c r="J20" s="7" t="s">
-        <v>87</v>
-      </c>
-      <c r="K20" s="7"/>
-    </row>
-    <row r="21" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.3">
+        <v>285</v>
+      </c>
+      <c r="K20" s="7" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" s="2" customFormat="1" ht="33" x14ac:dyDescent="0.3">
       <c r="A21" s="7" t="s">
-        <v>270</v>
+        <v>260</v>
       </c>
       <c r="B21" s="6" t="s">
         <v>129</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>181</v>
+        <v>171</v>
       </c>
       <c r="D21" s="6" t="s">
         <v>33</v>
@@ -4278,14 +4390,16 @@
       <c r="G21" s="7"/>
       <c r="H21" s="7"/>
       <c r="I21" s="7"/>
-      <c r="J21" s="7"/>
+      <c r="J21" s="7" t="s">
+        <v>279</v>
+      </c>
       <c r="K21" s="7" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.3">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" s="2" customFormat="1" ht="33" x14ac:dyDescent="0.3">
       <c r="A22" s="7" t="s">
-        <v>271</v>
+        <v>261</v>
       </c>
       <c r="B22" s="6" t="s">
         <v>129</v>
@@ -4305,26 +4419,28 @@
       <c r="G22" s="7"/>
       <c r="H22" s="7"/>
       <c r="I22" s="7"/>
-      <c r="J22" s="7"/>
+      <c r="J22" s="7" t="s">
+        <v>287</v>
+      </c>
       <c r="K22" s="7" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.3">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" s="2" customFormat="1" ht="165" x14ac:dyDescent="0.3">
       <c r="A23" s="16" t="s">
-        <v>254</v>
+        <v>244</v>
       </c>
       <c r="B23" s="17" t="s">
         <v>135</v>
       </c>
       <c r="C23" s="17" t="s">
-        <v>193</v>
+        <v>183</v>
       </c>
       <c r="D23" s="17" t="s">
         <v>140</v>
       </c>
       <c r="E23" s="16" t="s">
-        <v>194</v>
+        <v>184</v>
       </c>
       <c r="F23" s="16" t="s">
         <v>143</v>
@@ -4332,18 +4448,22 @@
       <c r="G23" s="16"/>
       <c r="H23" s="16"/>
       <c r="I23" s="16"/>
-      <c r="J23" s="16"/>
-      <c r="K23" s="16"/>
-    </row>
-    <row r="24" spans="1:11" s="2" customFormat="1" ht="33" x14ac:dyDescent="0.3">
+      <c r="J23" s="7" t="s">
+        <v>263</v>
+      </c>
+      <c r="K23" s="7" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" s="2" customFormat="1" ht="148.5" x14ac:dyDescent="0.3">
       <c r="A24" s="7" t="s">
-        <v>255</v>
+        <v>245</v>
       </c>
       <c r="B24" s="6" t="s">
         <v>135</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>195</v>
+        <v>185</v>
       </c>
       <c r="D24" s="6" t="s">
         <v>141</v>
@@ -4357,12 +4477,16 @@
       <c r="G24" s="7"/>
       <c r="H24" s="7"/>
       <c r="I24" s="7"/>
-      <c r="J24" s="7"/>
-      <c r="K24" s="7"/>
-    </row>
-    <row r="25" spans="1:11" s="2" customFormat="1" ht="33" x14ac:dyDescent="0.3">
+      <c r="J24" s="7" t="s">
+        <v>268</v>
+      </c>
+      <c r="K24" s="7" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" s="2" customFormat="1" ht="82.5" x14ac:dyDescent="0.3">
       <c r="A25" s="7" t="s">
-        <v>272</v>
+        <v>262</v>
       </c>
       <c r="B25" s="6" t="s">
         <v>135</v>
@@ -4374,7 +4498,7 @@
         <v>139</v>
       </c>
       <c r="E25" s="7" t="s">
-        <v>196</v>
+        <v>186</v>
       </c>
       <c r="F25" s="7" t="s">
         <v>146</v>
@@ -4382,12 +4506,16 @@
       <c r="G25" s="7"/>
       <c r="H25" s="7"/>
       <c r="I25" s="7"/>
-      <c r="J25" s="7"/>
-      <c r="K25" s="7"/>
-    </row>
-    <row r="26" spans="1:11" s="2" customFormat="1" ht="33" x14ac:dyDescent="0.3">
+      <c r="J25" s="7" t="s">
+        <v>276</v>
+      </c>
+      <c r="K25" s="7" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" s="2" customFormat="1" ht="82.5" x14ac:dyDescent="0.3">
       <c r="A26" s="7" t="s">
-        <v>258</v>
+        <v>248</v>
       </c>
       <c r="B26" s="6" t="s">
         <v>149</v>
@@ -4396,10 +4524,10 @@
         <v>102</v>
       </c>
       <c r="D26" s="6" t="s">
-        <v>197</v>
+        <v>187</v>
       </c>
       <c r="E26" s="7" t="s">
-        <v>198</v>
+        <v>188</v>
       </c>
       <c r="F26" s="7" t="s">
         <v>148</v>
@@ -4407,11 +4535,16 @@
       <c r="G26" s="7"/>
       <c r="H26" s="7"/>
       <c r="I26" s="7"/>
-      <c r="J26" s="7"/>
-      <c r="K26" s="7"/>
+      <c r="J26" s="7" t="s">
+        <v>285</v>
+      </c>
+      <c r="K26" s="7" t="s">
+        <v>286</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
[docs] upload security requirement & mitigation
upload security requirement & mitigation
</commit_message>
<xml_diff>
--- a/docs/05_threat_modeling/threat_modeling.xlsx
+++ b/docs/05_threat_modeling/threat_modeling.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git-dir\cmu_project\docs\05_threat_modeling\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\study\security\cmu\temp\cmu_project\docs\05_threat_modeling\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="676" uniqueCount="288">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="673" uniqueCount="285">
   <si>
     <t>Id</t>
   </si>
@@ -587,18 +587,6 @@
   </si>
   <si>
     <t>Network</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>Threat Level</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>Impact Level</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>Security Level</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
@@ -989,38 +977,12 @@
   <si>
     <t>User Credential Data should be encrypted in the storage.
 Use well-known cryptographic libraries and robust algorithms.</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>Encrypt user credential data in storage
-- Use OpenSSL library of latest version (1.1.1k)
-- Use an algorithm that are stronger than AES256
-- Use cbc of gcm mode
-Integrity Check with hash (optional when using cbc mode)
-- Use an alforithm that are stronger than sha256</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
     <t>the system shall know the change of the user credential data.
 The system must perform an integrity check before using user credentials.
 Use well-known cryptographic libraries and robust algorithms.</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>Integrity Check with hash functionan
-- Use OpenSSL library of latest version (1.1.1k)
-- Use an algorithm that are stronger than sha256
-Encrypt User credential (optional)
-- Use an algorithm that are stronger than AES256
-- Use cbc of gcm mode</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>Apply setting policy of cryptographically strong password
-- Enforce passwords longer than 10(?) characters.
-- Forces the use of mixed uppercase and lowercase letters of the alphabet
-Strong authentication method
-- Condider 2-Factor-Authentication method</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
@@ -1083,12 +1045,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>the system shall know the change of the user credential data.
-Server and client must communicate using an encrypted channel.
-Input validation check is required in Server side.</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>Input validation check is required in Server side.</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -1132,11 +1088,44 @@
     <t>Input validation check is required in Client side.</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
+  <si>
+    <t>the system shall know the change of the user credential data.
+Server and client must communicate using an encrypted channel.
+Input validation check is required in Server side.</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Encrypt user credential data in storage
+- Use OpenSSL library of latest version (1.1.1k)
+- Use an algorithm that are stronger than AES256
+- Use cbc of gcm mode
+Integrity Check with hash
+- Use an alforithm that are stronger than sha256</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Apply setting policy of cryptographically strong password
+- Enforce passwords longer than 7 characters.
+- Forces the use of mixed uppercase and lowercase letters of the alphabet
+Strong authentication method
+- Condider 2-Factor-Authentication method</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Integrity Check with hash function
+- Use OpenSSL library of latest version (1.1.1k)
+- Use an algorithm that are stronger than sha256
+Encrypt user credential data in storage
+- Use OpenSSL library of latest version (1.1.1k)
+- Use an algorithm that are stronger than AES256
+- Use cbc of gcm mode</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1798,7 +1787,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1857,9 +1846,6 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -2230,7 +2216,7 @@
     </row>
     <row r="2" spans="1:8" s="3" customFormat="1" ht="33" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>129</v>
@@ -2254,7 +2240,7 @@
     </row>
     <row r="3" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="B3" s="7" t="s">
         <v>129</v>
@@ -2278,7 +2264,7 @@
     </row>
     <row r="4" spans="1:8" s="2" customFormat="1" ht="33" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="B4" s="7" t="s">
         <v>129</v>
@@ -2302,7 +2288,7 @@
     </row>
     <row r="5" spans="1:8" s="2" customFormat="1" ht="33" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="B5" s="7" t="s">
         <v>129</v>
@@ -2326,7 +2312,7 @@
     </row>
     <row r="6" spans="1:8" s="2" customFormat="1" ht="33" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="B6" s="7" t="s">
         <v>129</v>
@@ -2350,7 +2336,7 @@
     </row>
     <row r="7" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="B7" s="7" t="s">
         <v>129</v>
@@ -2374,7 +2360,7 @@
     </row>
     <row r="8" spans="1:8" s="2" customFormat="1" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="B8" s="7" t="s">
         <v>129</v>
@@ -2398,7 +2384,7 @@
     </row>
     <row r="9" spans="1:8" s="2" customFormat="1" ht="33" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="B9" s="7" t="s">
         <v>129</v>
@@ -2422,7 +2408,7 @@
     </row>
     <row r="10" spans="1:8" s="10" customFormat="1" ht="33" x14ac:dyDescent="0.3">
       <c r="A10" s="9" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="B10" s="8" t="s">
         <v>129</v>
@@ -2448,7 +2434,7 @@
     </row>
     <row r="11" spans="1:8" s="2" customFormat="1" ht="33" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="B11" s="7" t="s">
         <v>129</v>
@@ -2472,7 +2458,7 @@
     </row>
     <row r="12" spans="1:8" s="10" customFormat="1" ht="33" x14ac:dyDescent="0.3">
       <c r="A12" s="9" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="B12" s="8" t="s">
         <v>129</v>
@@ -2498,7 +2484,7 @@
     </row>
     <row r="13" spans="1:8" s="10" customFormat="1" ht="33" x14ac:dyDescent="0.3">
       <c r="A13" s="9" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="B13" s="8" t="s">
         <v>129</v>
@@ -2524,7 +2510,7 @@
     </row>
     <row r="14" spans="1:8" s="2" customFormat="1" ht="33" x14ac:dyDescent="0.3">
       <c r="A14" s="7" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="B14" s="7" t="s">
         <v>129</v>
@@ -2550,7 +2536,7 @@
     </row>
     <row r="15" spans="1:8" s="10" customFormat="1" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A15" s="9" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="B15" s="8" t="s">
         <v>129</v>
@@ -2576,7 +2562,7 @@
     </row>
     <row r="16" spans="1:8" s="10" customFormat="1" ht="33" x14ac:dyDescent="0.3">
       <c r="A16" s="9" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="B16" s="8" t="s">
         <v>129</v>
@@ -2602,7 +2588,7 @@
     </row>
     <row r="17" spans="1:8" s="10" customFormat="1" ht="66" x14ac:dyDescent="0.3">
       <c r="A17" s="9" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="B17" s="8" t="s">
         <v>129</v>
@@ -2628,7 +2614,7 @@
     </row>
     <row r="18" spans="1:8" s="10" customFormat="1" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A18" s="9" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="B18" s="8" t="s">
         <v>129</v>
@@ -2654,7 +2640,7 @@
     </row>
     <row r="19" spans="1:8" s="10" customFormat="1" ht="82.5" x14ac:dyDescent="0.3">
       <c r="A19" s="9" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="B19" s="8" t="s">
         <v>129</v>
@@ -2680,7 +2666,7 @@
     </row>
     <row r="20" spans="1:8" s="10" customFormat="1" ht="33" x14ac:dyDescent="0.3">
       <c r="A20" s="9" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="B20" s="8" t="s">
         <v>129</v>
@@ -2706,7 +2692,7 @@
     </row>
     <row r="21" spans="1:8" s="10" customFormat="1" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A21" s="9" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="B21" s="8" t="s">
         <v>129</v>
@@ -2732,7 +2718,7 @@
     </row>
     <row r="22" spans="1:8" s="10" customFormat="1" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A22" s="9" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="B22" s="8" t="s">
         <v>129</v>
@@ -2758,7 +2744,7 @@
     </row>
     <row r="23" spans="1:8" s="10" customFormat="1" ht="33" x14ac:dyDescent="0.3">
       <c r="A23" s="9" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="B23" s="8" t="s">
         <v>129</v>
@@ -2784,7 +2770,7 @@
     </row>
     <row r="24" spans="1:8" s="10" customFormat="1" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A24" s="9" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="B24" s="8" t="s">
         <v>129</v>
@@ -2810,7 +2796,7 @@
     </row>
     <row r="25" spans="1:8" s="10" customFormat="1" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A25" s="9" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="B25" s="8" t="s">
         <v>129</v>
@@ -2836,7 +2822,7 @@
     </row>
     <row r="26" spans="1:8" s="10" customFormat="1" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A26" s="9" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="B26" s="8" t="s">
         <v>129</v>
@@ -2862,7 +2848,7 @@
     </row>
     <row r="27" spans="1:8" s="10" customFormat="1" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A27" s="9" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="B27" s="8" t="s">
         <v>129</v>
@@ -2888,7 +2874,7 @@
     </row>
     <row r="28" spans="1:8" s="10" customFormat="1" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A28" s="9" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="B28" s="8" t="s">
         <v>129</v>
@@ -2914,7 +2900,7 @@
     </row>
     <row r="29" spans="1:8" s="10" customFormat="1" ht="82.5" x14ac:dyDescent="0.3">
       <c r="A29" s="9" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="B29" s="8" t="s">
         <v>129</v>
@@ -2940,7 +2926,7 @@
     </row>
     <row r="30" spans="1:8" s="2" customFormat="1" ht="33" x14ac:dyDescent="0.3">
       <c r="A30" s="7" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="B30" s="6" t="s">
         <v>129</v>
@@ -2966,7 +2952,7 @@
     </row>
     <row r="31" spans="1:8" s="10" customFormat="1" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A31" s="9" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="B31" s="8" t="s">
         <v>129</v>
@@ -2992,7 +2978,7 @@
     </row>
     <row r="32" spans="1:8" s="10" customFormat="1" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A32" s="9" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="B32" s="8" t="s">
         <v>129</v>
@@ -3018,7 +3004,7 @@
     </row>
     <row r="33" spans="1:8" s="10" customFormat="1" ht="33" x14ac:dyDescent="0.3">
       <c r="A33" s="9" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="B33" s="8" t="s">
         <v>129</v>
@@ -3044,7 +3030,7 @@
     </row>
     <row r="34" spans="1:8" s="10" customFormat="1" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A34" s="9" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="B34" s="8" t="s">
         <v>129</v>
@@ -3070,7 +3056,7 @@
     </row>
     <row r="35" spans="1:8" s="2" customFormat="1" ht="33" x14ac:dyDescent="0.3">
       <c r="A35" s="7" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="B35" s="6" t="s">
         <v>129</v>
@@ -3096,7 +3082,7 @@
     </row>
     <row r="36" spans="1:8" s="2" customFormat="1" ht="33" x14ac:dyDescent="0.3">
       <c r="A36" s="7" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="B36" s="6" t="s">
         <v>129</v>
@@ -3120,7 +3106,7 @@
     </row>
     <row r="37" spans="1:8" s="10" customFormat="1" ht="82.5" x14ac:dyDescent="0.3">
       <c r="A37" s="9" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="B37" s="8" t="s">
         <v>129</v>
@@ -3146,7 +3132,7 @@
     </row>
     <row r="38" spans="1:8" s="10" customFormat="1" ht="115.5" x14ac:dyDescent="0.3">
       <c r="A38" s="9" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="B38" s="8" t="s">
         <v>129</v>
@@ -3172,7 +3158,7 @@
     </row>
     <row r="39" spans="1:8" s="10" customFormat="1" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A39" s="9" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="B39" s="8" t="s">
         <v>129</v>
@@ -3198,7 +3184,7 @@
     </row>
     <row r="40" spans="1:8" s="10" customFormat="1" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A40" s="9" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="B40" s="8" t="s">
         <v>129</v>
@@ -3224,7 +3210,7 @@
     </row>
     <row r="41" spans="1:8" s="10" customFormat="1" ht="66" x14ac:dyDescent="0.3">
       <c r="A41" s="9" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="B41" s="8" t="s">
         <v>129</v>
@@ -3250,7 +3236,7 @@
     </row>
     <row r="42" spans="1:8" s="2" customFormat="1" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A42" s="7" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="B42" s="6" t="s">
         <v>129</v>
@@ -3274,7 +3260,7 @@
     </row>
     <row r="43" spans="1:8" s="10" customFormat="1" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A43" s="9" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="B43" s="8" t="s">
         <v>129</v>
@@ -3300,7 +3286,7 @@
     </row>
     <row r="44" spans="1:8" s="10" customFormat="1" ht="33" x14ac:dyDescent="0.3">
       <c r="A44" s="9" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="B44" s="8" t="s">
         <v>129</v>
@@ -3326,7 +3312,7 @@
     </row>
     <row r="45" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A45" s="7" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="B45" s="6" t="s">
         <v>129</v>
@@ -3352,7 +3338,7 @@
     </row>
     <row r="46" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A46" s="7" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="B46" s="6" t="s">
         <v>129</v>
@@ -3376,7 +3362,7 @@
     </row>
     <row r="47" spans="1:8" s="2" customFormat="1" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A47" s="7" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="B47" s="6" t="s">
         <v>129</v>
@@ -3402,7 +3388,7 @@
     </row>
     <row r="48" spans="1:8" s="10" customFormat="1" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A48" s="9" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="B48" s="8" t="s">
         <v>129</v>
@@ -3428,7 +3414,7 @@
     </row>
     <row r="49" spans="1:8" s="2" customFormat="1" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A49" s="7" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="B49" s="6" t="s">
         <v>129</v>
@@ -3454,7 +3440,7 @@
     </row>
     <row r="50" spans="1:8" s="2" customFormat="1" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A50" s="7" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="B50" s="6" t="s">
         <v>129</v>
@@ -3478,7 +3464,7 @@
     </row>
     <row r="51" spans="1:8" s="10" customFormat="1" ht="33" x14ac:dyDescent="0.3">
       <c r="A51" s="9" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="B51" s="8" t="s">
         <v>129</v>
@@ -3504,7 +3490,7 @@
     </row>
     <row r="52" spans="1:8" s="10" customFormat="1" ht="33" x14ac:dyDescent="0.3">
       <c r="A52" s="9" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="B52" s="8" t="s">
         <v>129</v>
@@ -3530,7 +3516,7 @@
     </row>
     <row r="53" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A53" s="7" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="B53" s="6" t="s">
         <v>129</v>
@@ -3554,7 +3540,7 @@
     </row>
     <row r="54" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A54" s="7" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="B54" s="6" t="s">
         <v>129</v>
@@ -3578,7 +3564,7 @@
     </row>
     <row r="55" spans="1:8" s="10" customFormat="1" ht="99" x14ac:dyDescent="0.3">
       <c r="A55" s="9" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="B55" s="8" t="s">
         <v>129</v>
@@ -3604,7 +3590,7 @@
     </row>
     <row r="56" spans="1:8" s="10" customFormat="1" ht="99" x14ac:dyDescent="0.3">
       <c r="A56" s="9" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="B56" s="14" t="s">
         <v>129</v>
@@ -3640,7 +3626,7 @@
     </row>
     <row r="58" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A58" s="16" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="B58" s="17" t="s">
         <v>135</v>
@@ -3662,7 +3648,7 @@
     </row>
     <row r="59" spans="1:8" s="2" customFormat="1" ht="33" x14ac:dyDescent="0.3">
       <c r="A59" s="7" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="B59" s="6" t="s">
         <v>135</v>
@@ -3684,7 +3670,7 @@
     </row>
     <row r="60" spans="1:8" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A60" s="9" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="B60" s="8" t="s">
         <v>135</v>
@@ -3710,7 +3696,7 @@
     </row>
     <row r="61" spans="1:8" s="2" customFormat="1" ht="33" x14ac:dyDescent="0.3">
       <c r="A61" s="7" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="B61" s="6" t="s">
         <v>135</v>
@@ -3732,7 +3718,7 @@
     </row>
     <row r="63" spans="1:8" s="2" customFormat="1" ht="33" x14ac:dyDescent="0.3">
       <c r="A63" s="7" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="B63" s="6" t="s">
         <v>149</v>
@@ -3761,10 +3747,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K26"/>
+  <dimension ref="A1:H26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B25" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F34" sqref="F34"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -3775,14 +3761,11 @@
     <col min="4" max="4" width="36.125" customWidth="1"/>
     <col min="5" max="5" width="62" style="1" customWidth="1"/>
     <col min="6" max="6" width="35" customWidth="1"/>
-    <col min="7" max="7" width="11.875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="32" style="1" customWidth="1"/>
-    <col min="11" max="11" width="34.375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="32" style="1" customWidth="1"/>
+    <col min="8" max="8" width="34.375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -3801,63 +3784,51 @@
       <c r="F1" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="G1" s="20" t="s">
-        <v>151</v>
-      </c>
-      <c r="H1" s="20" t="s">
+      <c r="G1" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="H1" s="12" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" s="3" customFormat="1" ht="148.5" x14ac:dyDescent="0.3">
+      <c r="A2" s="7" t="s">
+        <v>186</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>153</v>
+      </c>
+      <c r="E2" s="7" t="s">
         <v>152</v>
-      </c>
-      <c r="I1" s="20" t="s">
-        <v>153</v>
-      </c>
-      <c r="J1" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="K1" s="12" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" s="3" customFormat="1" ht="165" x14ac:dyDescent="0.3">
-      <c r="A2" s="7" t="s">
-        <v>189</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>129</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>157</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>156</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>155</v>
       </c>
       <c r="F2" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="G2" s="7"/>
-      <c r="H2" s="7"/>
-      <c r="I2" s="7"/>
-      <c r="J2" s="7" t="s">
-        <v>263</v>
-      </c>
-      <c r="K2" s="7" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" s="2" customFormat="1" ht="148.5" x14ac:dyDescent="0.3">
+      <c r="G2" s="7" t="s">
+        <v>260</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" s="2" customFormat="1" ht="181.5" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="B3" s="7" t="s">
         <v>129</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="E3" s="7" t="s">
         <v>40</v>
@@ -3865,28 +3836,25 @@
       <c r="F3" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="G3" s="7"/>
-      <c r="H3" s="7"/>
-      <c r="I3" s="7"/>
-      <c r="J3" s="7" t="s">
-        <v>265</v>
-      </c>
-      <c r="K3" s="7" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" s="2" customFormat="1" ht="181.5" x14ac:dyDescent="0.3">
+      <c r="G3" s="7" t="s">
+        <v>261</v>
+      </c>
+      <c r="H3" s="7" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" s="2" customFormat="1" ht="181.5" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="B4" s="7" t="s">
         <v>129</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="E4" s="7" t="s">
         <v>41</v>
@@ -3894,57 +3862,51 @@
       <c r="F4" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="G4" s="7"/>
-      <c r="H4" s="7"/>
-      <c r="I4" s="7"/>
-      <c r="J4" s="7" t="s">
-        <v>278</v>
-      </c>
-      <c r="K4" s="7" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" s="2" customFormat="1" ht="148.5" x14ac:dyDescent="0.3">
+      <c r="G4" s="7" t="s">
+        <v>281</v>
+      </c>
+      <c r="H4" s="7" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" s="2" customFormat="1" ht="148.5" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="B5" s="7" t="s">
         <v>129</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="F5" s="7" t="s">
         <v>104</v>
       </c>
-      <c r="G5" s="7"/>
-      <c r="H5" s="7"/>
-      <c r="I5" s="7"/>
-      <c r="J5" s="7" t="s">
-        <v>268</v>
-      </c>
-      <c r="K5" s="7" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" s="2" customFormat="1" ht="66" x14ac:dyDescent="0.3">
+      <c r="G5" s="7" t="s">
+        <v>262</v>
+      </c>
+      <c r="H5" s="7" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" s="2" customFormat="1" ht="66" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="B6" s="7" t="s">
         <v>129</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="E6" s="7" t="s">
         <v>111</v>
@@ -3952,141 +3914,126 @@
       <c r="F6" s="7" t="s">
         <v>112</v>
       </c>
-      <c r="G6" s="7"/>
-      <c r="H6" s="7"/>
-      <c r="I6" s="7"/>
-      <c r="J6" s="7" t="s">
-        <v>269</v>
-      </c>
-      <c r="K6" s="7" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" s="2" customFormat="1" ht="132" x14ac:dyDescent="0.3">
+      <c r="G6" s="7" t="s">
+        <v>263</v>
+      </c>
+      <c r="H6" s="7" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" s="2" customFormat="1" ht="132" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="B7" s="7" t="s">
         <v>129</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="D7" s="6" t="s">
         <v>30</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="F7" s="7" t="s">
         <v>118</v>
       </c>
-      <c r="G7" s="7"/>
-      <c r="H7" s="7"/>
-      <c r="I7" s="7"/>
-      <c r="J7" s="7" t="s">
-        <v>272</v>
-      </c>
-      <c r="K7" s="7" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" s="2" customFormat="1" ht="66" x14ac:dyDescent="0.3">
+      <c r="G7" s="7" t="s">
+        <v>266</v>
+      </c>
+      <c r="H7" s="7" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" s="2" customFormat="1" ht="66" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="B8" s="7" t="s">
         <v>129</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="D8" s="6" t="s">
         <v>44</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="F8" s="7" t="s">
         <v>110</v>
       </c>
-      <c r="G8" s="7"/>
-      <c r="H8" s="7"/>
-      <c r="I8" s="7"/>
-      <c r="J8" s="7" t="s">
-        <v>274</v>
-      </c>
-      <c r="K8" s="7" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" s="2" customFormat="1" ht="148.5" x14ac:dyDescent="0.3">
+      <c r="G8" s="7" t="s">
+        <v>268</v>
+      </c>
+      <c r="H8" s="7" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" s="2" customFormat="1" ht="148.5" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="B9" s="7" t="s">
         <v>129</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="D9" s="6" t="s">
         <v>30</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="F9" s="7" t="s">
         <v>104</v>
       </c>
-      <c r="G9" s="7"/>
-      <c r="H9" s="7"/>
-      <c r="I9" s="7"/>
-      <c r="J9" s="7" t="s">
-        <v>275</v>
-      </c>
-      <c r="K9" s="7" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" s="2" customFormat="1" ht="82.5" x14ac:dyDescent="0.3">
+      <c r="G9" s="7" t="s">
+        <v>269</v>
+      </c>
+      <c r="H9" s="7" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" s="2" customFormat="1" ht="82.5" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="B10" s="7" t="s">
         <v>129</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="D10" s="6" t="s">
         <v>30</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>154</v>
-      </c>
-      <c r="G10" s="7"/>
-      <c r="H10" s="7"/>
-      <c r="I10" s="7"/>
-      <c r="J10" s="7" t="s">
-        <v>276</v>
-      </c>
-      <c r="K10" s="7" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" s="2" customFormat="1" ht="33" x14ac:dyDescent="0.3">
+        <v>151</v>
+      </c>
+      <c r="G10" s="7" t="s">
+        <v>270</v>
+      </c>
+      <c r="H10" s="7" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" s="2" customFormat="1" ht="33" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="B11" s="7" t="s">
         <v>129</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="D11" s="6" t="s">
         <v>30</v>
@@ -4097,115 +4044,103 @@
       <c r="F11" s="7" t="s">
         <v>122</v>
       </c>
-      <c r="G11" s="7"/>
-      <c r="H11" s="7"/>
-      <c r="I11" s="7"/>
-      <c r="J11" s="7" t="s">
-        <v>279</v>
-      </c>
-      <c r="K11" s="7" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" s="2" customFormat="1" ht="49.5" x14ac:dyDescent="0.3">
+      <c r="G11" s="7" t="s">
+        <v>272</v>
+      </c>
+      <c r="H11" s="7" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" s="2" customFormat="1" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="B12" s="6" t="s">
         <v>129</v>
       </c>
       <c r="C12" s="6" t="s">
+        <v>166</v>
+      </c>
+      <c r="D12" s="6" t="s">
         <v>169</v>
       </c>
-      <c r="D12" s="6" t="s">
-        <v>172</v>
-      </c>
       <c r="E12" s="7" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="F12" s="7" t="s">
         <v>116</v>
       </c>
-      <c r="G12" s="7"/>
-      <c r="H12" s="7"/>
-      <c r="I12" s="7"/>
-      <c r="J12" s="7" t="s">
-        <v>281</v>
-      </c>
-      <c r="K12" s="7" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" s="2" customFormat="1" ht="82.5" x14ac:dyDescent="0.3">
+      <c r="G12" s="7" t="s">
+        <v>274</v>
+      </c>
+      <c r="H12" s="7" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" s="2" customFormat="1" ht="82.5" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="B13" s="6" t="s">
         <v>129</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="F13" s="7" t="s">
         <v>114</v>
       </c>
-      <c r="G13" s="7"/>
-      <c r="H13" s="7"/>
-      <c r="I13" s="7"/>
-      <c r="J13" s="7" t="s">
-        <v>283</v>
-      </c>
-      <c r="K13" s="7" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" s="2" customFormat="1" ht="165" x14ac:dyDescent="0.3">
+      <c r="G13" s="7" t="s">
+        <v>276</v>
+      </c>
+      <c r="H13" s="7" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" s="2" customFormat="1" ht="148.5" x14ac:dyDescent="0.3">
       <c r="A14" s="7" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="B14" s="6" t="s">
         <v>129</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="D14" s="6" t="s">
         <v>31</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="F14" s="7" t="s">
         <v>115</v>
       </c>
-      <c r="G14" s="7"/>
-      <c r="H14" s="7"/>
-      <c r="I14" s="7"/>
-      <c r="J14" s="7" t="s">
-        <v>263</v>
-      </c>
-      <c r="K14" s="7" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" s="2" customFormat="1" ht="165" x14ac:dyDescent="0.3">
+      <c r="G14" s="7" t="s">
+        <v>260</v>
+      </c>
+      <c r="H14" s="7" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" s="2" customFormat="1" ht="148.5" x14ac:dyDescent="0.3">
       <c r="A15" s="7" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="B15" s="6" t="s">
         <v>129</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="E15" s="7" t="s">
         <v>76</v>
@@ -4213,19 +4148,16 @@
       <c r="F15" s="7" t="s">
         <v>115</v>
       </c>
-      <c r="G15" s="7"/>
-      <c r="H15" s="7"/>
-      <c r="I15" s="7"/>
-      <c r="J15" s="7" t="s">
-        <v>263</v>
-      </c>
-      <c r="K15" s="7" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" s="2" customFormat="1" ht="82.5" x14ac:dyDescent="0.3">
+      <c r="G15" s="7" t="s">
+        <v>260</v>
+      </c>
+      <c r="H15" s="7" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" s="2" customFormat="1" ht="82.5" x14ac:dyDescent="0.3">
       <c r="A16" s="7" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="B16" s="6" t="s">
         <v>129</v>
@@ -4234,7 +4166,7 @@
         <v>14</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="E16" s="7" t="s">
         <v>80</v>
@@ -4242,19 +4174,16 @@
       <c r="F16" s="7" t="s">
         <v>118</v>
       </c>
-      <c r="G16" s="7"/>
-      <c r="H16" s="7"/>
-      <c r="I16" s="7"/>
-      <c r="J16" s="7" t="s">
-        <v>276</v>
-      </c>
-      <c r="K16" s="7" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" s="2" customFormat="1" ht="82.5" x14ac:dyDescent="0.3">
+      <c r="G16" s="7" t="s">
+        <v>270</v>
+      </c>
+      <c r="H16" s="7" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" s="2" customFormat="1" ht="82.5" x14ac:dyDescent="0.3">
       <c r="A17" s="7" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="B17" s="6" t="s">
         <v>129</v>
@@ -4266,88 +4195,79 @@
         <v>33</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="F17" s="7" t="s">
         <v>118</v>
       </c>
-      <c r="G17" s="7"/>
-      <c r="H17" s="7"/>
-      <c r="I17" s="7"/>
-      <c r="J17" s="7" t="s">
-        <v>276</v>
-      </c>
-      <c r="K17" s="7" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" s="2" customFormat="1" ht="66" x14ac:dyDescent="0.3">
+      <c r="G17" s="7" t="s">
+        <v>270</v>
+      </c>
+      <c r="H17" s="7" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" s="2" customFormat="1" ht="66" x14ac:dyDescent="0.3">
       <c r="A18" s="7" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="B18" s="6" t="s">
         <v>129</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="D18" s="6" t="s">
         <v>33</v>
       </c>
       <c r="E18" s="7" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="F18" s="7" t="s">
         <v>123</v>
       </c>
-      <c r="G18" s="7"/>
-      <c r="H18" s="7"/>
-      <c r="I18" s="7"/>
-      <c r="J18" s="7" t="s">
+      <c r="G18" s="7" t="s">
         <v>124</v>
       </c>
-      <c r="K18" s="7" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" s="2" customFormat="1" ht="66" x14ac:dyDescent="0.3">
+      <c r="H18" s="7" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" s="2" customFormat="1" ht="66" x14ac:dyDescent="0.3">
       <c r="A19" s="7" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="B19" s="6" t="s">
         <v>129</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="D19" s="6" t="s">
         <v>33</v>
       </c>
       <c r="E19" s="7" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="F19" s="7" t="s">
         <v>126</v>
       </c>
-      <c r="G19" s="7"/>
-      <c r="H19" s="7"/>
-      <c r="I19" s="7"/>
-      <c r="J19" s="7" t="s">
+      <c r="G19" s="7" t="s">
         <v>124</v>
       </c>
-      <c r="K19" s="7" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" s="2" customFormat="1" ht="82.5" x14ac:dyDescent="0.3">
+      <c r="H19" s="7" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" s="2" customFormat="1" ht="82.5" x14ac:dyDescent="0.3">
       <c r="A20" s="7" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="B20" s="6" t="s">
         <v>129</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="D20" s="6" t="s">
         <v>33</v>
@@ -4358,25 +4278,22 @@
       <c r="F20" s="7" t="s">
         <v>128</v>
       </c>
-      <c r="G20" s="7"/>
-      <c r="H20" s="7"/>
-      <c r="I20" s="7"/>
-      <c r="J20" s="7" t="s">
-        <v>285</v>
-      </c>
-      <c r="K20" s="7" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" s="2" customFormat="1" ht="33" x14ac:dyDescent="0.3">
+      <c r="G20" s="7" t="s">
+        <v>278</v>
+      </c>
+      <c r="H20" s="7" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" s="2" customFormat="1" ht="33" x14ac:dyDescent="0.3">
       <c r="A21" s="7" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="B21" s="6" t="s">
         <v>129</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="D21" s="6" t="s">
         <v>33</v>
@@ -4387,19 +4304,16 @@
       <c r="F21" s="7" t="s">
         <v>127</v>
       </c>
-      <c r="G21" s="7"/>
-      <c r="H21" s="7"/>
-      <c r="I21" s="7"/>
-      <c r="J21" s="7" t="s">
-        <v>279</v>
-      </c>
-      <c r="K21" s="7" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" s="2" customFormat="1" ht="33" x14ac:dyDescent="0.3">
+      <c r="G21" s="7" t="s">
+        <v>272</v>
+      </c>
+      <c r="H21" s="7" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" s="2" customFormat="1" ht="33" x14ac:dyDescent="0.3">
       <c r="A22" s="7" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="B22" s="6" t="s">
         <v>129</v>
@@ -4416,54 +4330,48 @@
       <c r="F22" s="7" t="s">
         <v>127</v>
       </c>
-      <c r="G22" s="7"/>
-      <c r="H22" s="7"/>
-      <c r="I22" s="7"/>
-      <c r="J22" s="7" t="s">
-        <v>287</v>
-      </c>
-      <c r="K22" s="7" t="s">
+      <c r="G22" s="7" t="s">
         <v>280</v>
       </c>
-    </row>
-    <row r="23" spans="1:11" s="2" customFormat="1" ht="165" x14ac:dyDescent="0.3">
+      <c r="H22" s="7" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" s="2" customFormat="1" ht="148.5" x14ac:dyDescent="0.3">
       <c r="A23" s="16" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="B23" s="17" t="s">
         <v>135</v>
       </c>
       <c r="C23" s="17" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="D23" s="17" t="s">
         <v>140</v>
       </c>
       <c r="E23" s="16" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="F23" s="16" t="s">
         <v>143</v>
       </c>
-      <c r="G23" s="16"/>
-      <c r="H23" s="16"/>
-      <c r="I23" s="16"/>
-      <c r="J23" s="7" t="s">
-        <v>263</v>
-      </c>
-      <c r="K23" s="7" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" s="2" customFormat="1" ht="148.5" x14ac:dyDescent="0.3">
+      <c r="G23" s="7" t="s">
+        <v>260</v>
+      </c>
+      <c r="H23" s="7" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" s="2" customFormat="1" ht="148.5" x14ac:dyDescent="0.3">
       <c r="A24" s="7" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="B24" s="6" t="s">
         <v>135</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="D24" s="6" t="s">
         <v>141</v>
@@ -4474,19 +4382,16 @@
       <c r="F24" s="7" t="s">
         <v>144</v>
       </c>
-      <c r="G24" s="7"/>
-      <c r="H24" s="7"/>
-      <c r="I24" s="7"/>
-      <c r="J24" s="7" t="s">
-        <v>268</v>
-      </c>
-      <c r="K24" s="7" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" s="2" customFormat="1" ht="82.5" x14ac:dyDescent="0.3">
+      <c r="G24" s="7" t="s">
+        <v>262</v>
+      </c>
+      <c r="H24" s="7" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" s="2" customFormat="1" ht="82.5" x14ac:dyDescent="0.3">
       <c r="A25" s="7" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="B25" s="6" t="s">
         <v>135</v>
@@ -4498,24 +4403,21 @@
         <v>139</v>
       </c>
       <c r="E25" s="7" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="F25" s="7" t="s">
         <v>146</v>
       </c>
-      <c r="G25" s="7"/>
-      <c r="H25" s="7"/>
-      <c r="I25" s="7"/>
-      <c r="J25" s="7" t="s">
-        <v>276</v>
-      </c>
-      <c r="K25" s="7" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" s="2" customFormat="1" ht="82.5" x14ac:dyDescent="0.3">
+      <c r="G25" s="7" t="s">
+        <v>270</v>
+      </c>
+      <c r="H25" s="7" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" s="2" customFormat="1" ht="82.5" x14ac:dyDescent="0.3">
       <c r="A26" s="7" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="B26" s="6" t="s">
         <v>149</v>
@@ -4524,22 +4426,19 @@
         <v>102</v>
       </c>
       <c r="D26" s="6" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="E26" s="7" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="F26" s="7" t="s">
         <v>148</v>
       </c>
-      <c r="G26" s="7"/>
-      <c r="H26" s="7"/>
-      <c r="I26" s="7"/>
-      <c r="J26" s="7" t="s">
-        <v>285</v>
-      </c>
-      <c r="K26" s="7" t="s">
-        <v>286</v>
+      <c r="G26" s="7" t="s">
+        <v>278</v>
+      </c>
+      <c r="H26" s="7" t="s">
+        <v>279</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[docs] add item to threat_modeling
Add threat items related to certificates and keys.
</commit_message>
<xml_diff>
--- a/docs/05_threat_modeling/threat_modeling.xlsx
+++ b/docs/05_threat_modeling/threat_modeling.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\study\security\cmu\temp\cmu_project\docs\05_threat_modeling\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git-dir\cmu_project\docs\05_threat_modeling\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="673" uniqueCount="285">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="681" uniqueCount="292">
   <si>
     <t>Id</t>
   </si>
@@ -642,10 +642,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>Information Disclosure</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>Weak Authentification may lead to disclose information</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -690,10 +686,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>Tampering</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>Video Stream may be tampered with by an attacker.</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -703,10 +695,6 @@
   </si>
   <si>
     <t>Denial Of Service</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>Tampering</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
@@ -1121,11 +1109,55 @@
 - Consider mutual authentication between server and client</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
+  <si>
+    <t>TR-61</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Brainstorming</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Server &lt;=&gt; Client</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Tampering</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Spoofing</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Tampering/ Information Disclosure/ Spoofing</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>By changing the server/client's certificate or key, an attacker may attempt to connect to an unauthorized client.
+And attacker can try to steal the information of the encryption channel.</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>A server and client program must perform an integrity check before using a certificate or key.</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Need to protect or verify the certificates and keys used by the server and client</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Certificate &amp; Key file existance check
+Integrity Check with hash function
+- Use OpenSSL library of latest version (1.1.1k)
+- Use an algorithm that are stronger than sha256</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -2216,7 +2248,7 @@
     </row>
     <row r="2" spans="1:8" s="3" customFormat="1" ht="33" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>129</v>
@@ -2240,7 +2272,7 @@
     </row>
     <row r="3" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="B3" s="7" t="s">
         <v>129</v>
@@ -2264,7 +2296,7 @@
     </row>
     <row r="4" spans="1:8" s="2" customFormat="1" ht="33" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="B4" s="7" t="s">
         <v>129</v>
@@ -2288,7 +2320,7 @@
     </row>
     <row r="5" spans="1:8" s="2" customFormat="1" ht="33" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="B5" s="7" t="s">
         <v>129</v>
@@ -2312,7 +2344,7 @@
     </row>
     <row r="6" spans="1:8" s="2" customFormat="1" ht="33" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="B6" s="7" t="s">
         <v>129</v>
@@ -2336,7 +2368,7 @@
     </row>
     <row r="7" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="B7" s="7" t="s">
         <v>129</v>
@@ -2360,7 +2392,7 @@
     </row>
     <row r="8" spans="1:8" s="2" customFormat="1" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="B8" s="7" t="s">
         <v>129</v>
@@ -2384,7 +2416,7 @@
     </row>
     <row r="9" spans="1:8" s="2" customFormat="1" ht="33" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="B9" s="7" t="s">
         <v>129</v>
@@ -2408,7 +2440,7 @@
     </row>
     <row r="10" spans="1:8" s="10" customFormat="1" ht="33" x14ac:dyDescent="0.3">
       <c r="A10" s="9" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="B10" s="8" t="s">
         <v>129</v>
@@ -2434,7 +2466,7 @@
     </row>
     <row r="11" spans="1:8" s="2" customFormat="1" ht="33" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="B11" s="7" t="s">
         <v>129</v>
@@ -2458,7 +2490,7 @@
     </row>
     <row r="12" spans="1:8" s="10" customFormat="1" ht="33" x14ac:dyDescent="0.3">
       <c r="A12" s="9" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="B12" s="8" t="s">
         <v>129</v>
@@ -2484,7 +2516,7 @@
     </row>
     <row r="13" spans="1:8" s="10" customFormat="1" ht="33" x14ac:dyDescent="0.3">
       <c r="A13" s="9" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="B13" s="8" t="s">
         <v>129</v>
@@ -2510,7 +2542,7 @@
     </row>
     <row r="14" spans="1:8" s="2" customFormat="1" ht="33" x14ac:dyDescent="0.3">
       <c r="A14" s="7" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="B14" s="7" t="s">
         <v>129</v>
@@ -2536,7 +2568,7 @@
     </row>
     <row r="15" spans="1:8" s="10" customFormat="1" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A15" s="9" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="B15" s="8" t="s">
         <v>129</v>
@@ -2562,7 +2594,7 @@
     </row>
     <row r="16" spans="1:8" s="10" customFormat="1" ht="33" x14ac:dyDescent="0.3">
       <c r="A16" s="9" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="B16" s="8" t="s">
         <v>129</v>
@@ -2588,7 +2620,7 @@
     </row>
     <row r="17" spans="1:8" s="10" customFormat="1" ht="66" x14ac:dyDescent="0.3">
       <c r="A17" s="9" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="B17" s="8" t="s">
         <v>129</v>
@@ -2614,7 +2646,7 @@
     </row>
     <row r="18" spans="1:8" s="10" customFormat="1" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A18" s="9" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="B18" s="8" t="s">
         <v>129</v>
@@ -2640,7 +2672,7 @@
     </row>
     <row r="19" spans="1:8" s="10" customFormat="1" ht="82.5" x14ac:dyDescent="0.3">
       <c r="A19" s="9" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="B19" s="8" t="s">
         <v>129</v>
@@ -2666,7 +2698,7 @@
     </row>
     <row r="20" spans="1:8" s="10" customFormat="1" ht="33" x14ac:dyDescent="0.3">
       <c r="A20" s="9" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="B20" s="8" t="s">
         <v>129</v>
@@ -2692,7 +2724,7 @@
     </row>
     <row r="21" spans="1:8" s="10" customFormat="1" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A21" s="9" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="B21" s="8" t="s">
         <v>129</v>
@@ -2718,7 +2750,7 @@
     </row>
     <row r="22" spans="1:8" s="10" customFormat="1" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A22" s="9" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="B22" s="8" t="s">
         <v>129</v>
@@ -2744,7 +2776,7 @@
     </row>
     <row r="23" spans="1:8" s="10" customFormat="1" ht="33" x14ac:dyDescent="0.3">
       <c r="A23" s="9" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="B23" s="8" t="s">
         <v>129</v>
@@ -2770,7 +2802,7 @@
     </row>
     <row r="24" spans="1:8" s="10" customFormat="1" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A24" s="9" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="B24" s="8" t="s">
         <v>129</v>
@@ -2796,7 +2828,7 @@
     </row>
     <row r="25" spans="1:8" s="10" customFormat="1" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A25" s="9" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="B25" s="8" t="s">
         <v>129</v>
@@ -2822,7 +2854,7 @@
     </row>
     <row r="26" spans="1:8" s="10" customFormat="1" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A26" s="9" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="B26" s="8" t="s">
         <v>129</v>
@@ -2848,7 +2880,7 @@
     </row>
     <row r="27" spans="1:8" s="10" customFormat="1" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A27" s="9" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="B27" s="8" t="s">
         <v>129</v>
@@ -2874,7 +2906,7 @@
     </row>
     <row r="28" spans="1:8" s="10" customFormat="1" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A28" s="9" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="B28" s="8" t="s">
         <v>129</v>
@@ -2900,7 +2932,7 @@
     </row>
     <row r="29" spans="1:8" s="10" customFormat="1" ht="82.5" x14ac:dyDescent="0.3">
       <c r="A29" s="9" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="B29" s="8" t="s">
         <v>129</v>
@@ -2926,7 +2958,7 @@
     </row>
     <row r="30" spans="1:8" s="2" customFormat="1" ht="33" x14ac:dyDescent="0.3">
       <c r="A30" s="7" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="B30" s="6" t="s">
         <v>129</v>
@@ -2952,7 +2984,7 @@
     </row>
     <row r="31" spans="1:8" s="10" customFormat="1" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A31" s="9" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="B31" s="8" t="s">
         <v>129</v>
@@ -2978,7 +3010,7 @@
     </row>
     <row r="32" spans="1:8" s="10" customFormat="1" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A32" s="9" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="B32" s="8" t="s">
         <v>129</v>
@@ -3004,7 +3036,7 @@
     </row>
     <row r="33" spans="1:8" s="10" customFormat="1" ht="33" x14ac:dyDescent="0.3">
       <c r="A33" s="9" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="B33" s="8" t="s">
         <v>129</v>
@@ -3030,7 +3062,7 @@
     </row>
     <row r="34" spans="1:8" s="10" customFormat="1" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A34" s="9" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="B34" s="8" t="s">
         <v>129</v>
@@ -3056,7 +3088,7 @@
     </row>
     <row r="35" spans="1:8" s="2" customFormat="1" ht="33" x14ac:dyDescent="0.3">
       <c r="A35" s="7" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="B35" s="6" t="s">
         <v>129</v>
@@ -3082,7 +3114,7 @@
     </row>
     <row r="36" spans="1:8" s="2" customFormat="1" ht="33" x14ac:dyDescent="0.3">
       <c r="A36" s="7" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="B36" s="6" t="s">
         <v>129</v>
@@ -3106,7 +3138,7 @@
     </row>
     <row r="37" spans="1:8" s="10" customFormat="1" ht="82.5" x14ac:dyDescent="0.3">
       <c r="A37" s="9" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="B37" s="8" t="s">
         <v>129</v>
@@ -3132,7 +3164,7 @@
     </row>
     <row r="38" spans="1:8" s="10" customFormat="1" ht="115.5" x14ac:dyDescent="0.3">
       <c r="A38" s="9" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="B38" s="8" t="s">
         <v>129</v>
@@ -3158,7 +3190,7 @@
     </row>
     <row r="39" spans="1:8" s="10" customFormat="1" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A39" s="9" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="B39" s="8" t="s">
         <v>129</v>
@@ -3184,7 +3216,7 @@
     </row>
     <row r="40" spans="1:8" s="10" customFormat="1" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A40" s="9" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="B40" s="8" t="s">
         <v>129</v>
@@ -3210,7 +3242,7 @@
     </row>
     <row r="41" spans="1:8" s="10" customFormat="1" ht="66" x14ac:dyDescent="0.3">
       <c r="A41" s="9" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="B41" s="8" t="s">
         <v>129</v>
@@ -3236,7 +3268,7 @@
     </row>
     <row r="42" spans="1:8" s="2" customFormat="1" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A42" s="7" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="B42" s="6" t="s">
         <v>129</v>
@@ -3260,7 +3292,7 @@
     </row>
     <row r="43" spans="1:8" s="10" customFormat="1" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A43" s="9" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="B43" s="8" t="s">
         <v>129</v>
@@ -3286,7 +3318,7 @@
     </row>
     <row r="44" spans="1:8" s="10" customFormat="1" ht="33" x14ac:dyDescent="0.3">
       <c r="A44" s="9" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="B44" s="8" t="s">
         <v>129</v>
@@ -3312,7 +3344,7 @@
     </row>
     <row r="45" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A45" s="7" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="B45" s="6" t="s">
         <v>129</v>
@@ -3338,7 +3370,7 @@
     </row>
     <row r="46" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A46" s="7" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="B46" s="6" t="s">
         <v>129</v>
@@ -3362,7 +3394,7 @@
     </row>
     <row r="47" spans="1:8" s="2" customFormat="1" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A47" s="7" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="B47" s="6" t="s">
         <v>129</v>
@@ -3388,7 +3420,7 @@
     </row>
     <row r="48" spans="1:8" s="10" customFormat="1" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A48" s="9" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="B48" s="8" t="s">
         <v>129</v>
@@ -3414,7 +3446,7 @@
     </row>
     <row r="49" spans="1:8" s="2" customFormat="1" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A49" s="7" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="B49" s="6" t="s">
         <v>129</v>
@@ -3440,7 +3472,7 @@
     </row>
     <row r="50" spans="1:8" s="2" customFormat="1" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A50" s="7" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="B50" s="6" t="s">
         <v>129</v>
@@ -3464,7 +3496,7 @@
     </row>
     <row r="51" spans="1:8" s="10" customFormat="1" ht="33" x14ac:dyDescent="0.3">
       <c r="A51" s="9" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="B51" s="8" t="s">
         <v>129</v>
@@ -3490,7 +3522,7 @@
     </row>
     <row r="52" spans="1:8" s="10" customFormat="1" ht="33" x14ac:dyDescent="0.3">
       <c r="A52" s="9" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="B52" s="8" t="s">
         <v>129</v>
@@ -3516,7 +3548,7 @@
     </row>
     <row r="53" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A53" s="7" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="B53" s="6" t="s">
         <v>129</v>
@@ -3540,7 +3572,7 @@
     </row>
     <row r="54" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A54" s="7" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="B54" s="6" t="s">
         <v>129</v>
@@ -3564,7 +3596,7 @@
     </row>
     <row r="55" spans="1:8" s="10" customFormat="1" ht="99" x14ac:dyDescent="0.3">
       <c r="A55" s="9" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="B55" s="8" t="s">
         <v>129</v>
@@ -3590,7 +3622,7 @@
     </row>
     <row r="56" spans="1:8" s="10" customFormat="1" ht="99" x14ac:dyDescent="0.3">
       <c r="A56" s="9" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="B56" s="14" t="s">
         <v>129</v>
@@ -3626,7 +3658,7 @@
     </row>
     <row r="58" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A58" s="16" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="B58" s="17" t="s">
         <v>135</v>
@@ -3648,7 +3680,7 @@
     </row>
     <row r="59" spans="1:8" s="2" customFormat="1" ht="33" x14ac:dyDescent="0.3">
       <c r="A59" s="7" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="B59" s="6" t="s">
         <v>135</v>
@@ -3670,7 +3702,7 @@
     </row>
     <row r="60" spans="1:8" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A60" s="9" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="B60" s="8" t="s">
         <v>135</v>
@@ -3696,7 +3728,7 @@
     </row>
     <row r="61" spans="1:8" s="2" customFormat="1" ht="33" x14ac:dyDescent="0.3">
       <c r="A61" s="7" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="B61" s="6" t="s">
         <v>135</v>
@@ -3718,7 +3750,7 @@
     </row>
     <row r="63" spans="1:8" s="2" customFormat="1" ht="33" x14ac:dyDescent="0.3">
       <c r="A63" s="7" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="B63" s="6" t="s">
         <v>149</v>
@@ -3747,10 +3779,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H26"/>
+  <dimension ref="A1:H27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -3793,7 +3825,7 @@
     </row>
     <row r="2" spans="1:8" s="3" customFormat="1" ht="148.5" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>129</v>
@@ -3811,15 +3843,15 @@
         <v>105</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
     </row>
     <row r="3" spans="1:8" s="2" customFormat="1" ht="181.5" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="B3" s="7" t="s">
         <v>129</v>
@@ -3837,15 +3869,15 @@
         <v>105</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="H3" s="7" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
     </row>
     <row r="4" spans="1:8" s="2" customFormat="1" ht="181.5" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="B4" s="7" t="s">
         <v>129</v>
@@ -3863,15 +3895,15 @@
         <v>105</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="H4" s="7" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
     </row>
     <row r="5" spans="1:8" s="2" customFormat="1" ht="148.5" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="B5" s="7" t="s">
         <v>129</v>
@@ -3889,15 +3921,15 @@
         <v>104</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="H5" s="7" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
     </row>
     <row r="6" spans="1:8" s="2" customFormat="1" ht="66" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="B6" s="7" t="s">
         <v>129</v>
@@ -3915,15 +3947,15 @@
         <v>112</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="H6" s="7" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
     </row>
     <row r="7" spans="1:8" s="2" customFormat="1" ht="132" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="B7" s="7" t="s">
         <v>129</v>
@@ -3941,15 +3973,15 @@
         <v>118</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="H7" s="7" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
     </row>
     <row r="8" spans="1:8" s="2" customFormat="1" ht="66" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="B8" s="7" t="s">
         <v>129</v>
@@ -3967,73 +3999,73 @@
         <v>110</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="H8" s="7" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
     </row>
     <row r="9" spans="1:8" s="2" customFormat="1" ht="148.5" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="B9" s="7" t="s">
         <v>129</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>164</v>
+        <v>137</v>
       </c>
       <c r="D9" s="6" t="s">
         <v>30</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="F9" s="7" t="s">
         <v>104</v>
       </c>
       <c r="G9" s="7" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="H9" s="7" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
     </row>
     <row r="10" spans="1:8" s="2" customFormat="1" ht="82.5" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="B10" s="7" t="s">
         <v>129</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D10" s="6" t="s">
         <v>30</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="F10" s="7" t="s">
         <v>151</v>
       </c>
       <c r="G10" s="7" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="H10" s="7" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
     </row>
     <row r="11" spans="1:8" s="2" customFormat="1" ht="33" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="B11" s="7" t="s">
         <v>129</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D11" s="6" t="s">
         <v>30</v>
@@ -4045,67 +4077,67 @@
         <v>122</v>
       </c>
       <c r="G11" s="7" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="H11" s="7" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
     </row>
     <row r="12" spans="1:8" s="2" customFormat="1" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="B12" s="6" t="s">
         <v>129</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D12" s="6" t="s">
+        <v>168</v>
+      </c>
+      <c r="E12" s="7" t="s">
         <v>169</v>
-      </c>
-      <c r="E12" s="7" t="s">
-        <v>170</v>
       </c>
       <c r="F12" s="7" t="s">
         <v>116</v>
       </c>
       <c r="G12" s="7" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="H12" s="7" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
     </row>
     <row r="13" spans="1:8" s="2" customFormat="1" ht="82.5" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="B13" s="6" t="s">
         <v>129</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D13" s="6" t="s">
+        <v>170</v>
+      </c>
+      <c r="E13" s="7" t="s">
         <v>171</v>
-      </c>
-      <c r="E13" s="7" t="s">
-        <v>172</v>
       </c>
       <c r="F13" s="7" t="s">
         <v>114</v>
       </c>
       <c r="G13" s="7" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="H13" s="7" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
     </row>
     <row r="14" spans="1:8" s="2" customFormat="1" ht="148.5" x14ac:dyDescent="0.3">
       <c r="A14" s="7" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="B14" s="6" t="s">
         <v>129</v>
@@ -4117,21 +4149,21 @@
         <v>31</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="F14" s="7" t="s">
         <v>115</v>
       </c>
       <c r="G14" s="7" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="H14" s="7" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
     </row>
     <row r="15" spans="1:8" s="2" customFormat="1" ht="148.5" x14ac:dyDescent="0.3">
       <c r="A15" s="7" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="B15" s="6" t="s">
         <v>129</v>
@@ -4140,7 +4172,7 @@
         <v>156</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E15" s="7" t="s">
         <v>76</v>
@@ -4149,15 +4181,15 @@
         <v>115</v>
       </c>
       <c r="G15" s="7" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="H15" s="7" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
     </row>
     <row r="16" spans="1:8" s="2" customFormat="1" ht="82.5" x14ac:dyDescent="0.3">
       <c r="A16" s="7" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="B16" s="6" t="s">
         <v>129</v>
@@ -4166,7 +4198,7 @@
         <v>14</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E16" s="7" t="s">
         <v>80</v>
@@ -4175,53 +4207,53 @@
         <v>118</v>
       </c>
       <c r="G16" s="7" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="H16" s="7" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
     </row>
     <row r="17" spans="1:8" s="2" customFormat="1" ht="82.5" x14ac:dyDescent="0.3">
       <c r="A17" s="7" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="B17" s="6" t="s">
         <v>129</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>14</v>
+        <v>286</v>
       </c>
       <c r="D17" s="6" t="s">
         <v>33</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="F17" s="7" t="s">
         <v>118</v>
       </c>
       <c r="G17" s="7" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="H17" s="7" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
     </row>
     <row r="18" spans="1:8" s="2" customFormat="1" ht="66" x14ac:dyDescent="0.3">
       <c r="A18" s="7" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="B18" s="6" t="s">
         <v>129</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>176</v>
+        <v>136</v>
       </c>
       <c r="D18" s="6" t="s">
         <v>33</v>
       </c>
       <c r="E18" s="7" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="F18" s="7" t="s">
         <v>123</v>
@@ -4230,12 +4262,12 @@
         <v>124</v>
       </c>
       <c r="H18" s="7" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
     </row>
     <row r="19" spans="1:8" s="2" customFormat="1" ht="66" x14ac:dyDescent="0.3">
       <c r="A19" s="7" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="B19" s="6" t="s">
         <v>129</v>
@@ -4247,7 +4279,7 @@
         <v>33</v>
       </c>
       <c r="E19" s="7" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="F19" s="7" t="s">
         <v>126</v>
@@ -4256,18 +4288,18 @@
         <v>124</v>
       </c>
       <c r="H19" s="7" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
     </row>
     <row r="20" spans="1:8" s="2" customFormat="1" ht="82.5" x14ac:dyDescent="0.3">
       <c r="A20" s="7" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="B20" s="6" t="s">
         <v>129</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D20" s="6" t="s">
         <v>33</v>
@@ -4279,21 +4311,21 @@
         <v>128</v>
       </c>
       <c r="G20" s="7" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="H20" s="7" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
     </row>
     <row r="21" spans="1:8" s="2" customFormat="1" ht="33" x14ac:dyDescent="0.3">
       <c r="A21" s="7" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="B21" s="6" t="s">
         <v>129</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D21" s="6" t="s">
         <v>33</v>
@@ -4305,15 +4337,15 @@
         <v>127</v>
       </c>
       <c r="G21" s="7" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="H21" s="7" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
     </row>
     <row r="22" spans="1:8" s="2" customFormat="1" ht="33" x14ac:dyDescent="0.3">
       <c r="A22" s="7" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="B22" s="6" t="s">
         <v>129</v>
@@ -4331,47 +4363,47 @@
         <v>127</v>
       </c>
       <c r="G22" s="7" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="H22" s="7" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
     </row>
     <row r="23" spans="1:8" s="2" customFormat="1" ht="148.5" x14ac:dyDescent="0.3">
       <c r="A23" s="16" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="B23" s="17" t="s">
         <v>135</v>
       </c>
       <c r="C23" s="17" t="s">
-        <v>180</v>
+        <v>285</v>
       </c>
       <c r="D23" s="17" t="s">
         <v>140</v>
       </c>
       <c r="E23" s="16" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="F23" s="16" t="s">
         <v>143</v>
       </c>
       <c r="G23" s="7" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="H23" s="7" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
     </row>
     <row r="24" spans="1:8" s="2" customFormat="1" ht="148.5" x14ac:dyDescent="0.3">
       <c r="A24" s="7" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="B24" s="6" t="s">
         <v>135</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="D24" s="6" t="s">
         <v>141</v>
@@ -4383,15 +4415,15 @@
         <v>144</v>
       </c>
       <c r="G24" s="7" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="H24" s="7" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
     </row>
     <row r="25" spans="1:8" s="2" customFormat="1" ht="82.5" x14ac:dyDescent="0.3">
       <c r="A25" s="7" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="B25" s="6" t="s">
         <v>135</v>
@@ -4403,21 +4435,21 @@
         <v>139</v>
       </c>
       <c r="E25" s="7" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="F25" s="7" t="s">
         <v>146</v>
       </c>
       <c r="G25" s="7" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="H25" s="7" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
     </row>
     <row r="26" spans="1:8" s="2" customFormat="1" ht="82.5" x14ac:dyDescent="0.3">
       <c r="A26" s="7" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="B26" s="6" t="s">
         <v>149</v>
@@ -4426,19 +4458,45 @@
         <v>102</v>
       </c>
       <c r="D26" s="6" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="E26" s="7" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="F26" s="7" t="s">
         <v>148</v>
       </c>
       <c r="G26" s="7" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="H26" s="7" t="s">
-        <v>278</v>
+        <v>275</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="99" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>282</v>
+      </c>
+      <c r="B27" t="s">
+        <v>283</v>
+      </c>
+      <c r="C27" t="s">
+        <v>287</v>
+      </c>
+      <c r="D27" t="s">
+        <v>284</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="F27" t="s">
+        <v>290</v>
+      </c>
+      <c r="G27" t="s">
+        <v>289</v>
+      </c>
+      <c r="H27" s="1" t="s">
+        <v>291</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[docs] modify item for threat_modeling
modify review of item
</commit_message>
<xml_diff>
--- a/docs/05_threat_modeling/threat_modeling.xlsx
+++ b/docs/05_threat_modeling/threat_modeling.xlsx
@@ -1134,23 +1134,23 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>By changing the server/client's certificate or key, an attacker may attempt to connect to an unauthorized client.
-And attacker can try to steal the information of the encryption channel.</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>A server and client program must perform an integrity check before using a certificate or key.</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>Need to protect or verify the certificates and keys used by the server and client</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>Certificate &amp; Key file existance check
 Integrity Check with hash function
 - Use OpenSSL library of latest version (1.1.1k)
 - Use an algorithm that are stronger than sha256</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Need to protect or verify the certificates and keys used by the server and client for TLS communication</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>By changing the server/client's certificate or key, an attacker may attempt to connect to an unauthorized client.
+And attacker can try to steal the information of the encryption channel.</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>A server and client program must perform an integrity check before using a certificate or key.</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -4487,16 +4487,16 @@
         <v>284</v>
       </c>
       <c r="E27" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="F27" t="s">
+        <v>289</v>
+      </c>
+      <c r="G27" t="s">
+        <v>291</v>
+      </c>
+      <c r="H27" s="1" t="s">
         <v>288</v>
-      </c>
-      <c r="F27" t="s">
-        <v>290</v>
-      </c>
-      <c r="G27" t="s">
-        <v>289</v>
-      </c>
-      <c r="H27" s="1" t="s">
-        <v>291</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[docs] update threat and requirement
update threat and requirement
</commit_message>
<xml_diff>
--- a/docs/05_threat_modeling/threat_modeling.xlsx
+++ b/docs/05_threat_modeling/threat_modeling.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git-dir\cmu_project\docs\05_threat_modeling\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\study\security\cmu\temp\cmu_project\docs\05_threat_modeling\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="681" uniqueCount="292">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="687" uniqueCount="291">
   <si>
     <t>Id</t>
   </si>
@@ -1110,11 +1110,19 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
+    <t>Tampering</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Spoofing</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
     <t>TR-61</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>Brainstorming</t>
+    <t>Tampering/ Information Disclosure/ Spoofing</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
@@ -1122,15 +1130,16 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>Tampering</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>Spoofing</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>Tampering/ Information Disclosure/ Spoofing</t>
+    <t>By changing the server/client's certificate or key, an attacker may attempt to connect to an unauthorized client.
+And attacker can try to steal the information of the encryption channel.</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Need to protect or verify the certificates and keys used by the server and client for TLS communication</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>A server and client program must perform an integrity check before using a certificate or key.</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
@@ -1140,24 +1149,11 @@
 - Use an algorithm that are stronger than sha256</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
-  <si>
-    <t>Need to protect or verify the certificates and keys used by the server and client for TLS communication</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>By changing the server/client's certificate or key, an attacker may attempt to connect to an unauthorized client.
-And attacker can try to steal the information of the encryption channel.</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>A server and client program must perform an integrity check before using a certificate or key.</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -2201,11 +2197,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H63"/>
+  <dimension ref="A1:H64"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
+      <pane ySplit="1" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D67" sqref="D67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -3770,6 +3766,28 @@
       <c r="G63" s="7"/>
       <c r="H63" s="7"/>
     </row>
+    <row r="64" spans="1:8" s="2" customFormat="1" ht="49.5" x14ac:dyDescent="0.3">
+      <c r="A64" s="7" t="s">
+        <v>284</v>
+      </c>
+      <c r="B64" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="C64" s="6" t="s">
+        <v>285</v>
+      </c>
+      <c r="D64" s="6" t="s">
+        <v>286</v>
+      </c>
+      <c r="E64" s="7" t="s">
+        <v>287</v>
+      </c>
+      <c r="F64" s="7" t="s">
+        <v>288</v>
+      </c>
+      <c r="G64" s="7"/>
+      <c r="H64" s="7"/>
+    </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3781,8 +3799,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G29" sqref="G29"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -4221,7 +4239,7 @@
         <v>129</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="D17" s="6" t="s">
         <v>33</v>
@@ -4377,7 +4395,7 @@
         <v>135</v>
       </c>
       <c r="C23" s="17" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="D23" s="17" t="s">
         <v>140</v>
@@ -4473,30 +4491,30 @@
         <v>275</v>
       </c>
     </row>
-    <row r="27" spans="1:8" ht="99" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
-        <v>282</v>
-      </c>
-      <c r="B27" t="s">
-        <v>283</v>
-      </c>
-      <c r="C27" t="s">
+    <row r="27" spans="1:8" s="2" customFormat="1" ht="99" x14ac:dyDescent="0.3">
+      <c r="A27" s="7" t="s">
+        <v>284</v>
+      </c>
+      <c r="B27" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="C27" s="6" t="s">
+        <v>285</v>
+      </c>
+      <c r="D27" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="E27" s="7" t="s">
         <v>287</v>
       </c>
-      <c r="D27" t="s">
-        <v>284</v>
-      </c>
-      <c r="E27" s="1" t="s">
+      <c r="F27" s="7" t="s">
+        <v>288</v>
+      </c>
+      <c r="G27" s="7" t="s">
+        <v>289</v>
+      </c>
+      <c r="H27" s="7" t="s">
         <v>290</v>
-      </c>
-      <c r="F27" t="s">
-        <v>289</v>
-      </c>
-      <c r="G27" t="s">
-        <v>291</v>
-      </c>
-      <c r="H27" s="1" t="s">
-        <v>288</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[docs] add items for threat_modeling
threats related to face recognition data
threats related to cryptographic key management
</commit_message>
<xml_diff>
--- a/docs/05_threat_modeling/threat_modeling.xlsx
+++ b/docs/05_threat_modeling/threat_modeling.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\study\security\cmu\temp\cmu_project\docs\05_threat_modeling\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git-dir\cmu_project\docs\05_threat_modeling\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="687" uniqueCount="291">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="703" uniqueCount="307">
   <si>
     <t>Id</t>
   </si>
@@ -1149,11 +1149,92 @@
 - Use an algorithm that are stronger than sha256</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
+  <si>
+    <t>TR-62</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Brainstorming</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Brainstorming</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Tampering/ Information Disclosure</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Face Recognition data</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>By modifying the face recognition data, an attacker may cause an error or abnormal operation in the face recognition result.
+By stealing facial recognition data, an attacker can steal information from the system.</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Need to protect face recognition data</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>User Credential Data should be encrypted in the storage.
+Use well-known cryptographic libraries and robust algorithms.</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Face recognition data should be encrypted in the storage.
+Use well-known cryptographic libraries and robust algorithms.</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Encrypt face recongnition data in storage
+- Use OpenSSL library of latest version (1.1.1k)
+- Use an algorithm that are stronger than AES256
+- Use cbc of gcm mode
+Integrity Check with hash
+- Use an alforithm that are stronger than sha256</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>TR-63</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Cryptographically robust</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Need to preventing reverse analysis of encrypted information
+Need to protect ROOT encrypt key
+</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Use random encrypt key
+- use TRNG (True Random Number Generator) is best
+- Cryptographically secure pseudorandom number generator can be used alternatively
+Protect ROOT encrytpion key
+- HSM (Hardware Secure Module) is best
+- alternatively White-box Cryptography or Code obfuscation methon can be used</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Every enctyption time, newly generated random key is used for encryption to make reverse analysis difficult
+ROOT encrypt key must be protected from binary analysis</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>An attacker can find out the ROOT KEY used for encryption through reverse binary analysis, decrypt the encrypted file, and steal information.
+An attacker can infer the key used for encryption through statistical analysis of the encrypted file.</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1815,7 +1896,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1874,6 +1955,12 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="11" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -3797,10 +3884,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H27"/>
+  <dimension ref="A1:H29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G27" sqref="G27"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -4173,7 +4260,7 @@
         <v>115</v>
       </c>
       <c r="G14" s="7" t="s">
-        <v>257</v>
+        <v>298</v>
       </c>
       <c r="H14" s="7" t="s">
         <v>277</v>
@@ -4496,7 +4583,7 @@
         <v>284</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>149</v>
+        <v>292</v>
       </c>
       <c r="C27" s="6" t="s">
         <v>285</v>
@@ -4515,6 +4602,58 @@
       </c>
       <c r="H27" s="7" t="s">
         <v>290</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" ht="165" x14ac:dyDescent="0.3">
+      <c r="A28" s="20" t="s">
+        <v>291</v>
+      </c>
+      <c r="B28" s="21" t="s">
+        <v>293</v>
+      </c>
+      <c r="C28" s="21" t="s">
+        <v>294</v>
+      </c>
+      <c r="D28" s="21" t="s">
+        <v>295</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="F28" s="20" t="s">
+        <v>297</v>
+      </c>
+      <c r="G28" s="7" t="s">
+        <v>299</v>
+      </c>
+      <c r="H28" s="7" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="198" x14ac:dyDescent="0.3">
+      <c r="A29" s="20" t="s">
+        <v>301</v>
+      </c>
+      <c r="B29" s="21" t="s">
+        <v>293</v>
+      </c>
+      <c r="C29" s="21" t="s">
+        <v>102</v>
+      </c>
+      <c r="D29" s="21" t="s">
+        <v>302</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>305</v>
+      </c>
+      <c r="H29" s="1" t="s">
+        <v>304</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[docs] fix wrong word in threat_modeling files
fix wrong word in threat_modeling files
</commit_message>
<xml_diff>
--- a/docs/05_threat_modeling/threat_modeling.xlsx
+++ b/docs/05_threat_modeling/threat_modeling.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="703" uniqueCount="307">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="703" uniqueCount="309">
   <si>
     <t>Id</t>
   </si>
@@ -1066,30 +1066,11 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>Encrypt user credential data in storage
-- Use OpenSSL library of latest version (1.1.1k)
-- Use an algorithm that are stronger than AES256
-- Use cbc of gcm mode
-Integrity Check with hash
-- Use an alforithm that are stronger than sha256</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>Apply setting policy of cryptographically strong password
 - Enforce passwords longer than 7 characters.
 - Forces the use of mixed uppercase and lowercase letters of the alphabet
 Strong authentication method
 - Condider 2-Factor-Authentication method</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>Integrity Check with hash function
-- Use OpenSSL library of latest version (1.1.1k)
-- Use an algorithm that are stronger than sha256
-Encrypt user credential data in storage
-- Use OpenSSL library of latest version (1.1.1k)
-- Use an algorithm that are stronger than AES256
-- Use cbc of gcm mode</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
@@ -1189,15 +1170,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>Encrypt face recongnition data in storage
-- Use OpenSSL library of latest version (1.1.1k)
-- Use an algorithm that are stronger than AES256
-- Use cbc of gcm mode
-Integrity Check with hash
-- Use an alforithm that are stronger than sha256</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>TR-63</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -1228,6 +1200,52 @@
   <si>
     <t>An attacker can find out the ROOT KEY used for encryption through reverse binary analysis, decrypt the encrypted file, and steal information.
 An attacker can infer the key used for encryption through statistical analysis of the encrypted file.</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Encrypt user credential data in storage
+- Use OpenSSL library of latest version (1.1.1k)
+- Use an algorithm that are stronger than AES256
+- Use cbc or gcm mode
+Integrity Check with hash
+- Use an alforithm that are stronger than sha256</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Encrypt user credential data in storage
+- Use OpenSSL library of latest version (1.1.1k)
+- Use an algorithm that are stronger than AES256
+- Use cbc or gcm mode
+Integrity Check with hash
+- Use an alforithm that are stronger than sha256</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Integrity Check with hash function
+- Use OpenSSL library of latest version (1.1.1k)
+- Use an algorithm that are stronger than sha256
+Encrypt user credential data in storage
+- Use OpenSSL library of latest version (1.1.1k)
+- Use an algorithm that are stronger than AES256
+- Use cbc or gcm mode</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Encrypt user credential data in storage
+- Use OpenSSL library of latest version (1.1.1k)
+- Use an algorithm that are stronger than AES256
+- Use cbc or gcm mode
+Integrity Check with hash
+- Use an alforithm that are stronger than sha256</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Encrypt face recongnition data in storage
+- Use OpenSSL library of latest version (1.1.1k)
+- Use an algorithm that are stronger than AES256
+- Use cbc or gcm mode
+Integrity Check with hash
+- Use an alforithm that are stronger than sha256</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -3855,22 +3873,22 @@
     </row>
     <row r="64" spans="1:8" s="2" customFormat="1" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A64" s="7" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="B64" s="6" t="s">
         <v>149</v>
       </c>
       <c r="C64" s="6" t="s">
+        <v>283</v>
+      </c>
+      <c r="D64" s="6" t="s">
+        <v>284</v>
+      </c>
+      <c r="E64" s="7" t="s">
         <v>285</v>
       </c>
-      <c r="D64" s="6" t="s">
+      <c r="F64" s="7" t="s">
         <v>286</v>
-      </c>
-      <c r="E64" s="7" t="s">
-        <v>287</v>
-      </c>
-      <c r="F64" s="7" t="s">
-        <v>288</v>
       </c>
       <c r="G64" s="7"/>
       <c r="H64" s="7"/>
@@ -3887,7 +3905,7 @@
   <dimension ref="A1:H29"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A25" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+      <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -3951,7 +3969,7 @@
         <v>257</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>277</v>
+        <v>304</v>
       </c>
     </row>
     <row r="3" spans="1:8" s="2" customFormat="1" ht="181.5" x14ac:dyDescent="0.3">
@@ -3977,7 +3995,7 @@
         <v>258</v>
       </c>
       <c r="H3" s="7" t="s">
-        <v>279</v>
+        <v>306</v>
       </c>
     </row>
     <row r="4" spans="1:8" s="2" customFormat="1" ht="181.5" x14ac:dyDescent="0.3">
@@ -4000,10 +4018,10 @@
         <v>105</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="H4" s="7" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
     </row>
     <row r="5" spans="1:8" s="2" customFormat="1" ht="148.5" x14ac:dyDescent="0.3">
@@ -4029,7 +4047,7 @@
         <v>259</v>
       </c>
       <c r="H5" s="7" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="6" spans="1:8" s="2" customFormat="1" ht="66" x14ac:dyDescent="0.3">
@@ -4133,7 +4151,7 @@
         <v>265</v>
       </c>
       <c r="H9" s="7" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="10" spans="1:8" s="2" customFormat="1" ht="82.5" x14ac:dyDescent="0.3">
@@ -4260,10 +4278,10 @@
         <v>115</v>
       </c>
       <c r="G14" s="7" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="H14" s="7" t="s">
-        <v>277</v>
+        <v>305</v>
       </c>
     </row>
     <row r="15" spans="1:8" s="2" customFormat="1" ht="148.5" x14ac:dyDescent="0.3">
@@ -4289,7 +4307,7 @@
         <v>257</v>
       </c>
       <c r="H15" s="7" t="s">
-        <v>277</v>
+        <v>304</v>
       </c>
     </row>
     <row r="16" spans="1:8" s="2" customFormat="1" ht="82.5" x14ac:dyDescent="0.3">
@@ -4326,7 +4344,7 @@
         <v>129</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="D17" s="6" t="s">
         <v>33</v>
@@ -4482,7 +4500,7 @@
         <v>135</v>
       </c>
       <c r="C23" s="17" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="D23" s="17" t="s">
         <v>140</v>
@@ -4497,7 +4515,7 @@
         <v>257</v>
       </c>
       <c r="H23" s="7" t="s">
-        <v>277</v>
+        <v>307</v>
       </c>
     </row>
     <row r="24" spans="1:8" s="2" customFormat="1" ht="148.5" x14ac:dyDescent="0.3">
@@ -4523,7 +4541,7 @@
         <v>259</v>
       </c>
       <c r="H24" s="7" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="25" spans="1:8" s="2" customFormat="1" ht="82.5" x14ac:dyDescent="0.3">
@@ -4580,80 +4598,80 @@
     </row>
     <row r="27" spans="1:8" s="2" customFormat="1" ht="99" x14ac:dyDescent="0.3">
       <c r="A27" s="7" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="D27" s="6" t="s">
         <v>139</v>
       </c>
       <c r="E27" s="7" t="s">
+        <v>285</v>
+      </c>
+      <c r="F27" s="7" t="s">
+        <v>286</v>
+      </c>
+      <c r="G27" s="7" t="s">
         <v>287</v>
       </c>
-      <c r="F27" s="7" t="s">
+      <c r="H27" s="7" t="s">
         <v>288</v>
-      </c>
-      <c r="G27" s="7" t="s">
-        <v>289</v>
-      </c>
-      <c r="H27" s="7" t="s">
-        <v>290</v>
       </c>
     </row>
     <row r="28" spans="1:8" ht="165" x14ac:dyDescent="0.3">
       <c r="A28" s="20" t="s">
+        <v>289</v>
+      </c>
+      <c r="B28" s="21" t="s">
         <v>291</v>
       </c>
-      <c r="B28" s="21" t="s">
+      <c r="C28" s="21" t="s">
+        <v>292</v>
+      </c>
+      <c r="D28" s="21" t="s">
         <v>293</v>
       </c>
-      <c r="C28" s="21" t="s">
+      <c r="E28" s="1" t="s">
         <v>294</v>
       </c>
-      <c r="D28" s="21" t="s">
+      <c r="F28" s="20" t="s">
         <v>295</v>
       </c>
-      <c r="E28" s="1" t="s">
-        <v>296</v>
-      </c>
-      <c r="F28" s="20" t="s">
+      <c r="G28" s="7" t="s">
         <v>297</v>
       </c>
-      <c r="G28" s="7" t="s">
-        <v>299</v>
-      </c>
       <c r="H28" s="7" t="s">
-        <v>300</v>
+        <v>308</v>
       </c>
     </row>
     <row r="29" spans="1:8" ht="198" x14ac:dyDescent="0.3">
       <c r="A29" s="20" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="B29" s="21" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="C29" s="21" t="s">
         <v>102</v>
       </c>
       <c r="D29" s="21" t="s">
+        <v>299</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="G29" s="1" t="s">
         <v>302</v>
       </c>
-      <c r="E29" s="1" t="s">
-        <v>306</v>
-      </c>
-      <c r="F29" s="1" t="s">
-        <v>303</v>
-      </c>
-      <c r="G29" s="1" t="s">
-        <v>305</v>
-      </c>
       <c r="H29" s="1" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[docs] update 2 threats
update 2 threats
</commit_message>
<xml_diff>
--- a/docs/05_threat_modeling/threat_modeling.xlsx
+++ b/docs/05_threat_modeling/threat_modeling.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git-dir\cmu_project\docs\05_threat_modeling\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\study\security\cmu\temp\cmu_project\docs\05_threat_modeling\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="703" uniqueCount="309">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="715" uniqueCount="314">
   <si>
     <t>Id</t>
   </si>
@@ -1063,14 +1063,6 @@
   </si>
   <si>
     <t>Input validation check is required in Client side.</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>Apply setting policy of cryptographically strong password
-- Enforce passwords longer than 7 characters.
-- Forces the use of mixed uppercase and lowercase letters of the alphabet
-Strong authentication method
-- Condider 2-Factor-Authentication method</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
@@ -1248,11 +1240,37 @@
 - Use an alforithm that are stronger than sha256</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
+  <si>
+    <t>Tampering/ Information Disclosure</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>N/A</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>TR-62</t>
+  </si>
+  <si>
+    <t>TR-63</t>
+  </si>
+  <si>
+    <t>Face Recognition data</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Apply setting policy of cryptographically strong password
+- Enforce passwords longer than 7 characters.
+- Forces the use of mixed the letters of the alphabet and numbers.
+Strong authentication method
+- Condider 2-Factor-Authentication method</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1914,7 +1932,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1973,12 +1991,6 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="11" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -2302,11 +2314,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H64"/>
+  <dimension ref="A1:H66"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D67" sqref="D67"/>
+      <pane ySplit="1" topLeftCell="A56" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A64" sqref="A64:H66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -3873,25 +3885,69 @@
     </row>
     <row r="64" spans="1:8" s="2" customFormat="1" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A64" s="7" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B64" s="6" t="s">
         <v>149</v>
       </c>
       <c r="C64" s="6" t="s">
+        <v>282</v>
+      </c>
+      <c r="D64" s="6" t="s">
         <v>283</v>
       </c>
-      <c r="D64" s="6" t="s">
+      <c r="E64" s="7" t="s">
         <v>284</v>
       </c>
-      <c r="E64" s="7" t="s">
+      <c r="F64" s="7" t="s">
         <v>285</v>
-      </c>
-      <c r="F64" s="7" t="s">
-        <v>286</v>
       </c>
       <c r="G64" s="7"/>
       <c r="H64" s="7"/>
+    </row>
+    <row r="65" spans="1:8" s="2" customFormat="1" ht="66" x14ac:dyDescent="0.3">
+      <c r="A65" s="7" t="s">
+        <v>310</v>
+      </c>
+      <c r="B65" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="C65" s="6" t="s">
+        <v>308</v>
+      </c>
+      <c r="D65" s="6" t="s">
+        <v>292</v>
+      </c>
+      <c r="E65" s="7" t="s">
+        <v>293</v>
+      </c>
+      <c r="F65" s="7" t="s">
+        <v>294</v>
+      </c>
+      <c r="G65" s="7"/>
+      <c r="H65" s="7"/>
+    </row>
+    <row r="66" spans="1:8" s="2" customFormat="1" ht="82.5" x14ac:dyDescent="0.3">
+      <c r="A66" s="7" t="s">
+        <v>311</v>
+      </c>
+      <c r="B66" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="C66" s="6" t="s">
+        <v>309</v>
+      </c>
+      <c r="D66" s="6" t="s">
+        <v>298</v>
+      </c>
+      <c r="E66" s="7" t="s">
+        <v>302</v>
+      </c>
+      <c r="F66" s="7" t="s">
+        <v>299</v>
+      </c>
+      <c r="G66" s="7"/>
+      <c r="H66" s="7"/>
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
@@ -3905,7 +3961,7 @@
   <dimension ref="A1:H29"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A25" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H27" sqref="H27"/>
+      <selection activeCell="H26" sqref="H26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -3969,7 +4025,7 @@
         <v>257</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="3" spans="1:8" s="2" customFormat="1" ht="181.5" x14ac:dyDescent="0.3">
@@ -3995,7 +4051,7 @@
         <v>258</v>
       </c>
       <c r="H3" s="7" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="4" spans="1:8" s="2" customFormat="1" ht="181.5" x14ac:dyDescent="0.3">
@@ -4018,10 +4074,10 @@
         <v>105</v>
       </c>
       <c r="G4" s="7" t="s">
+        <v>277</v>
+      </c>
+      <c r="H4" s="7" t="s">
         <v>278</v>
-      </c>
-      <c r="H4" s="7" t="s">
-        <v>279</v>
       </c>
     </row>
     <row r="5" spans="1:8" s="2" customFormat="1" ht="148.5" x14ac:dyDescent="0.3">
@@ -4047,7 +4103,7 @@
         <v>259</v>
       </c>
       <c r="H5" s="7" t="s">
-        <v>277</v>
+        <v>313</v>
       </c>
     </row>
     <row r="6" spans="1:8" s="2" customFormat="1" ht="66" x14ac:dyDescent="0.3">
@@ -4151,7 +4207,7 @@
         <v>265</v>
       </c>
       <c r="H9" s="7" t="s">
-        <v>277</v>
+        <v>313</v>
       </c>
     </row>
     <row r="10" spans="1:8" s="2" customFormat="1" ht="82.5" x14ac:dyDescent="0.3">
@@ -4278,10 +4334,10 @@
         <v>115</v>
       </c>
       <c r="G14" s="7" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="H14" s="7" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="15" spans="1:8" s="2" customFormat="1" ht="148.5" x14ac:dyDescent="0.3">
@@ -4307,7 +4363,7 @@
         <v>257</v>
       </c>
       <c r="H15" s="7" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="16" spans="1:8" s="2" customFormat="1" ht="82.5" x14ac:dyDescent="0.3">
@@ -4344,7 +4400,7 @@
         <v>129</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="D17" s="6" t="s">
         <v>33</v>
@@ -4500,7 +4556,7 @@
         <v>135</v>
       </c>
       <c r="C23" s="17" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D23" s="17" t="s">
         <v>140</v>
@@ -4515,7 +4571,7 @@
         <v>257</v>
       </c>
       <c r="H23" s="7" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="24" spans="1:8" s="2" customFormat="1" ht="148.5" x14ac:dyDescent="0.3">
@@ -4541,7 +4597,7 @@
         <v>259</v>
       </c>
       <c r="H24" s="7" t="s">
-        <v>277</v>
+        <v>313</v>
       </c>
     </row>
     <row r="25" spans="1:8" s="2" customFormat="1" ht="82.5" x14ac:dyDescent="0.3">
@@ -4598,80 +4654,80 @@
     </row>
     <row r="27" spans="1:8" s="2" customFormat="1" ht="99" x14ac:dyDescent="0.3">
       <c r="A27" s="7" t="s">
+        <v>281</v>
+      </c>
+      <c r="B27" s="6" t="s">
+        <v>289</v>
+      </c>
+      <c r="C27" s="6" t="s">
         <v>282</v>
-      </c>
-      <c r="B27" s="6" t="s">
-        <v>290</v>
-      </c>
-      <c r="C27" s="6" t="s">
-        <v>283</v>
       </c>
       <c r="D27" s="6" t="s">
         <v>139</v>
       </c>
       <c r="E27" s="7" t="s">
+        <v>284</v>
+      </c>
+      <c r="F27" s="7" t="s">
         <v>285</v>
       </c>
-      <c r="F27" s="7" t="s">
+      <c r="G27" s="7" t="s">
         <v>286</v>
       </c>
-      <c r="G27" s="7" t="s">
+      <c r="H27" s="7" t="s">
         <v>287</v>
       </c>
-      <c r="H27" s="7" t="s">
+    </row>
+    <row r="28" spans="1:8" s="2" customFormat="1" ht="165" x14ac:dyDescent="0.3">
+      <c r="A28" s="7" t="s">
         <v>288</v>
       </c>
-    </row>
-    <row r="28" spans="1:8" ht="165" x14ac:dyDescent="0.3">
-      <c r="A28" s="20" t="s">
-        <v>289</v>
-      </c>
-      <c r="B28" s="21" t="s">
+      <c r="B28" s="6" t="s">
+        <v>290</v>
+      </c>
+      <c r="C28" s="6" t="s">
         <v>291</v>
       </c>
-      <c r="C28" s="21" t="s">
-        <v>292</v>
-      </c>
-      <c r="D28" s="21" t="s">
+      <c r="D28" s="6" t="s">
+        <v>312</v>
+      </c>
+      <c r="E28" s="7" t="s">
         <v>293</v>
       </c>
-      <c r="E28" s="1" t="s">
+      <c r="F28" s="7" t="s">
         <v>294</v>
       </c>
-      <c r="F28" s="20" t="s">
-        <v>295</v>
-      </c>
       <c r="G28" s="7" t="s">
+        <v>296</v>
+      </c>
+      <c r="H28" s="7" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" s="2" customFormat="1" ht="198" x14ac:dyDescent="0.3">
+      <c r="A29" s="7" t="s">
         <v>297</v>
       </c>
-      <c r="H28" s="7" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" ht="198" x14ac:dyDescent="0.3">
-      <c r="A29" s="20" t="s">
+      <c r="B29" s="6" t="s">
+        <v>290</v>
+      </c>
+      <c r="C29" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="D29" s="6" t="s">
         <v>298</v>
       </c>
-      <c r="B29" s="21" t="s">
-        <v>291</v>
-      </c>
-      <c r="C29" s="21" t="s">
-        <v>102</v>
-      </c>
-      <c r="D29" s="21" t="s">
+      <c r="E29" s="7" t="s">
+        <v>302</v>
+      </c>
+      <c r="F29" s="7" t="s">
         <v>299</v>
       </c>
-      <c r="E29" s="1" t="s">
-        <v>303</v>
-      </c>
-      <c r="F29" s="1" t="s">
+      <c r="G29" s="7" t="s">
+        <v>301</v>
+      </c>
+      <c r="H29" s="7" t="s">
         <v>300</v>
-      </c>
-      <c r="G29" s="1" t="s">
-        <v>302</v>
-      </c>
-      <c r="H29" s="1" t="s">
-        <v>301</v>
       </c>
     </row>
   </sheetData>

</xml_diff>